<commit_message>
analysiss finish with no car names
</commit_message>
<xml_diff>
--- a/outputs/analysiss.xlsx
+++ b/outputs/analysiss.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,35 +472,40 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RENT-MOTORS-06-12-23</t>
+          <t>RENT-MOTORS-22-02-24</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>REX-RENT-06-12-23</t>
+          <t>REX-RENT-22-02-24</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>A-ARENDA-06-12-23</t>
+          <t>A-ARENDA-22-02-24</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>STORLET-06-12-23</t>
+          <t>ALMAK-22-02-24</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>STORLET-22-02-24</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DELTA</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>DELTA %</t>
         </is>
@@ -526,13 +531,14 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
         <v>1750</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>488.9000000000001</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>21.84</v>
       </c>
     </row>
@@ -552,13 +558,14 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
         <v>1750</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>377.5499999999997</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>17.75</v>
       </c>
     </row>
@@ -578,13 +585,14 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
         <v>1500</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>515.3499999999999</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>25.57</v>
       </c>
     </row>
@@ -604,13 +612,14 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
         <v>1500</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>358.95</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>19.31</v>
       </c>
     </row>
@@ -630,13 +639,14 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
         <v>1500</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>246.75</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>14.13</v>
       </c>
     </row>
@@ -656,13 +666,14 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
         <v>1450</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>229.5999999999999</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>13.67</v>
       </c>
     </row>
@@ -684,13 +695,14 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
         <v>2798.2</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
       <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -708,13 +720,14 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
         <v>2658.8</v>
       </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
       <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -732,13 +745,14 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
         <v>2518.55</v>
       </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
       <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -756,13 +770,14 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
         <v>2323.05</v>
       </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
       <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -780,13 +795,14 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" t="n">
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
         <v>2182.8</v>
       </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
       <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -804,13 +820,14 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" t="n">
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="n">
         <v>2098.65</v>
       </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
       <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -832,13 +849,14 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
         <v>0</v>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
@@ -854,13 +872,14 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
         <v>0</v>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
@@ -876,13 +895,14 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="n">
         <v>0</v>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
@@ -898,13 +918,14 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
@@ -920,13 +941,14 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>0</v>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
@@ -942,13 +964,14 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="n">
-        <v>0</v>
-      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
         <v>0</v>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -967,14 +990,17 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="n">
+      <c r="G20" t="n">
+        <v>3470</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="n">
         <v>3280.15</v>
       </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
       <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -991,14 +1017,17 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="n">
+      <c r="G21" t="n">
+        <v>3270</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="n">
         <v>3116.95</v>
       </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
       <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1015,14 +1044,17 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="n">
+      <c r="G22" t="n">
+        <v>2970</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="n">
         <v>2952.9</v>
       </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
       <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1039,14 +1071,17 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="n">
+      <c r="G23" t="n">
+        <v>2970</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="n">
         <v>2624.8</v>
       </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
       <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1063,14 +1098,17 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="n">
+      <c r="G24" t="n">
+        <v>2870</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="n">
         <v>2296.7</v>
       </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
       <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1087,14 +1125,17 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="n">
+      <c r="G25" t="n">
+        <v>2870</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="n">
         <v>2296.7</v>
       </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
       <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1116,13 +1157,14 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="n">
         <v>2431.85</v>
       </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
       <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1140,13 +1182,14 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
-      <c r="H27" t="n">
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="n">
         <v>2310.3</v>
       </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
       <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1164,13 +1207,14 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" t="n">
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="n">
         <v>2188.75</v>
       </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
       <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1188,13 +1232,14 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="n">
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="n">
         <v>2018.75</v>
       </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
       <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1212,13 +1257,14 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
-      <c r="H30" t="n">
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="n">
         <v>1897.2</v>
       </c>
-      <c r="I30" t="n">
-        <v>0</v>
-      </c>
       <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1236,13 +1282,14 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
-      <c r="H31" t="n">
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="n">
         <v>1824.1</v>
       </c>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
       <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1263,18 +1310,23 @@
       <c r="D32" t="n">
         <v>2200</v>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>3200</v>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="n">
-        <v>2000</v>
+        <v>2570</v>
       </c>
       <c r="H32" t="n">
         <v>2000</v>
       </c>
       <c r="I32" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J32" t="n">
         <v>1039.6</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>34.2</v>
       </c>
     </row>
@@ -1291,18 +1343,23 @@
       <c r="D33" t="n">
         <v>2200</v>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="n">
+        <v>2816.67</v>
+      </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
-        <v>2000</v>
+        <v>2470</v>
       </c>
       <c r="H33" t="n">
         <v>2000</v>
       </c>
       <c r="I33" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J33" t="n">
         <v>888.2999999999997</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>30.76</v>
       </c>
     </row>
@@ -1319,18 +1376,23 @@
       <c r="D34" t="n">
         <v>1900</v>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="n">
+        <v>2321.43</v>
+      </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>1800</v>
+        <v>2270</v>
       </c>
       <c r="H34" t="n">
         <v>1800</v>
       </c>
       <c r="I34" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J34" t="n">
         <v>936.1500000000001</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>34.21</v>
       </c>
     </row>
@@ -1347,18 +1409,23 @@
       <c r="D35" t="n">
         <v>1900</v>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>2285.71</v>
+      </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
-        <v>1800</v>
+        <v>2270</v>
       </c>
       <c r="H35" t="n">
         <v>1800</v>
       </c>
       <c r="I35" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J35" t="n">
         <v>723.6500000000001</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>28.67</v>
       </c>
     </row>
@@ -1375,18 +1442,23 @@
       <c r="D36" t="n">
         <v>1900</v>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>2273.81</v>
+      </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
-        <v>1500</v>
+        <v>2170</v>
       </c>
       <c r="H36" t="n">
         <v>1500</v>
       </c>
       <c r="I36" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J36" t="n">
         <v>871.5</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>36.75</v>
       </c>
     </row>
@@ -1403,18 +1475,23 @@
       <c r="D37" t="n">
         <v>1800</v>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>2216.67</v>
+      </c>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="n">
-        <v>1500</v>
+        <v>2170</v>
       </c>
       <c r="H37" t="n">
         <v>1500</v>
       </c>
       <c r="I37" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J37" t="n">
         <v>779.6999999999998</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>34.2</v>
       </c>
     </row>
@@ -1436,13 +1513,14 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
-      <c r="H38" t="n">
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
         <v>2809.25</v>
       </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
       <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1460,13 +1538,14 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
-      <c r="H39" t="n">
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
         <v>2669</v>
       </c>
-      <c r="I39" t="n">
-        <v>0</v>
-      </c>
       <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1484,13 +1563,14 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
-      <c r="H40" t="n">
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
         <v>2528.75</v>
       </c>
-      <c r="I40" t="n">
-        <v>0</v>
-      </c>
       <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1508,13 +1588,14 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
-      <c r="H41" t="n">
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
         <v>2247.4</v>
       </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
       <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1532,13 +1613,14 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="n">
         <v>1966.9</v>
       </c>
-      <c r="I42" t="n">
-        <v>0</v>
-      </c>
       <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1556,13 +1638,14 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="n">
         <v>1966.9</v>
       </c>
-      <c r="I43" t="n">
-        <v>0</v>
-      </c>
       <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1581,20 +1664,21 @@
         <v>3511.35</v>
       </c>
       <c r="D44" t="inlineStr"/>
-      <c r="E44" t="n">
-        <v>3900</v>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>1800</v>
+        <v>2570</v>
       </c>
       <c r="H44" t="n">
         <v>1800</v>
       </c>
       <c r="I44" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J44" t="n">
         <v>1711.35</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>48.74</v>
       </c>
     </row>
@@ -1609,20 +1693,21 @@
         <v>3336.25</v>
       </c>
       <c r="D45" t="inlineStr"/>
-      <c r="E45" t="n">
-        <v>2600</v>
-      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
-        <v>1800</v>
+        <v>2470</v>
       </c>
       <c r="H45" t="n">
         <v>1800</v>
       </c>
       <c r="I45" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J45" t="n">
         <v>1536.25</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>46.05</v>
       </c>
     </row>
@@ -1637,20 +1722,21 @@
         <v>3160.3</v>
       </c>
       <c r="D46" t="inlineStr"/>
-      <c r="E46" t="n">
-        <v>2164.29</v>
-      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="n">
-        <v>1600</v>
+        <v>2270</v>
       </c>
       <c r="H46" t="n">
         <v>1600</v>
       </c>
       <c r="I46" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J46" t="n">
         <v>1560.3</v>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>49.37</v>
       </c>
     </row>
@@ -1665,20 +1751,21 @@
         <v>2809.25</v>
       </c>
       <c r="D47" t="inlineStr"/>
-      <c r="E47" t="n">
-        <v>2057.14</v>
-      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
-        <v>1600</v>
+        <v>2270</v>
       </c>
       <c r="H47" t="n">
         <v>1600</v>
       </c>
       <c r="I47" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J47" t="n">
         <v>1209.25</v>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>43.05</v>
       </c>
     </row>
@@ -1693,20 +1780,21 @@
         <v>2458.2</v>
       </c>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="n">
-        <v>2021.43</v>
-      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="n">
-        <v>1400</v>
+        <v>2170</v>
       </c>
       <c r="H48" t="n">
         <v>1400</v>
       </c>
       <c r="I48" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J48" t="n">
         <v>1058.2</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>43.05</v>
       </c>
     </row>
@@ -1721,20 +1809,21 @@
         <v>2458.2</v>
       </c>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="n">
-        <v>1950</v>
-      </c>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="n">
-        <v>1400</v>
+        <v>2170</v>
       </c>
       <c r="H49" t="n">
         <v>1400</v>
       </c>
       <c r="I49" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J49" t="n">
         <v>1058.2</v>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>43.05</v>
       </c>
     </row>
@@ -1752,19 +1841,22 @@
       <c r="C50" t="n">
         <v>3136.5</v>
       </c>
-      <c r="D50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>3000</v>
+      </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="n">
-        <v>1800</v>
-      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
         <v>1800</v>
       </c>
       <c r="I50" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J50" t="n">
         <v>1336.5</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>42.61</v>
       </c>
     </row>
@@ -1778,19 +1870,22 @@
       <c r="C51" t="n">
         <v>2980.1</v>
       </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>3000</v>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
-      <c r="G51" t="n">
-        <v>1800</v>
-      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
         <v>1800</v>
       </c>
       <c r="I51" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J51" t="n">
         <v>1180.1</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>39.6</v>
       </c>
     </row>
@@ -1804,19 +1899,22 @@
       <c r="C52" t="n">
         <v>2822.85</v>
       </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>2600</v>
+      </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
-      <c r="G52" t="n">
-        <v>1600</v>
-      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
         <v>1600</v>
       </c>
       <c r="I52" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J52" t="n">
         <v>1222.85</v>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>43.32</v>
       </c>
     </row>
@@ -1830,19 +1928,22 @@
       <c r="C53" t="n">
         <v>2509.2</v>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>2600</v>
+      </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
-      <c r="G53" t="n">
-        <v>1600</v>
-      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
         <v>1600</v>
       </c>
       <c r="I53" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J53" t="n">
         <v>909.1999999999998</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>36.23</v>
       </c>
     </row>
@@ -1856,19 +1957,22 @@
       <c r="C54" t="n">
         <v>2195.55</v>
       </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>2600</v>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
-      <c r="G54" t="n">
-        <v>1200</v>
-      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
         <v>1200</v>
       </c>
       <c r="I54" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J54" t="n">
         <v>995.5499999999997</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>45.34</v>
       </c>
     </row>
@@ -1882,19 +1986,22 @@
       <c r="C55" t="n">
         <v>2195.55</v>
       </c>
-      <c r="D55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>2100</v>
+      </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
-      <c r="G55" t="n">
-        <v>1200</v>
-      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
         <v>1200</v>
       </c>
       <c r="I55" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J55" t="n">
         <v>995.5499999999997</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>45.34</v>
       </c>
     </row>
@@ -1914,19 +2021,20 @@
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>6456</v>
+        <v>6055</v>
       </c>
       <c r="F56" t="inlineStr"/>
-      <c r="G56" t="n">
-        <v>2100</v>
-      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
         <v>2100</v>
       </c>
       <c r="I56" t="n">
+        <v>2100</v>
+      </c>
+      <c r="J56" t="n">
         <v>1589.85</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>43.09</v>
       </c>
     </row>
@@ -1942,19 +2050,20 @@
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>4991.33</v>
+        <v>5721.67</v>
       </c>
       <c r="F57" t="inlineStr"/>
-      <c r="G57" t="n">
-        <v>2100</v>
-      </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
         <v>2100</v>
       </c>
       <c r="I57" t="n">
+        <v>2100</v>
+      </c>
+      <c r="J57" t="n">
         <v>1405.4</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>40.09</v>
       </c>
     </row>
@@ -1970,19 +2079,20 @@
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>3639.43</v>
+        <v>5076.43</v>
       </c>
       <c r="F58" t="inlineStr"/>
-      <c r="G58" t="n">
-        <v>1900</v>
-      </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
         <v>1900</v>
       </c>
       <c r="I58" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J58" t="n">
         <v>1420.95</v>
       </c>
-      <c r="J58" t="n">
+      <c r="K58" t="n">
         <v>42.79</v>
       </c>
     </row>
@@ -1998,19 +2108,20 @@
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>3403.64</v>
+        <v>5040.71</v>
       </c>
       <c r="F59" t="inlineStr"/>
-      <c r="G59" t="n">
-        <v>1900</v>
-      </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
         <v>1900</v>
       </c>
       <c r="I59" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J59" t="n">
         <v>1052.05</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>35.64</v>
       </c>
     </row>
@@ -2026,19 +2137,20 @@
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>3280.76</v>
+        <v>5028.81</v>
       </c>
       <c r="F60" t="inlineStr"/>
-      <c r="G60" t="n">
-        <v>1500</v>
-      </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
         <v>1500</v>
       </c>
       <c r="I60" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J60" t="n">
         <v>1083.15</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>41.93</v>
       </c>
     </row>
@@ -2054,19 +2166,20 @@
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>3005.4</v>
+        <v>4471.67</v>
       </c>
       <c r="F61" t="inlineStr"/>
-      <c r="G61" t="n">
-        <v>1500</v>
-      </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
         <v>1500</v>
       </c>
       <c r="I61" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J61" t="n">
         <v>1083.15</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
         <v>41.93</v>
       </c>
     </row>
@@ -2085,22 +2198,25 @@
         <v>4250.849999999999</v>
       </c>
       <c r="D62" t="n">
-        <v>3000</v>
+        <v>3800</v>
       </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="n">
-        <v>3700</v>
+        <v>3510</v>
       </c>
       <c r="G62" t="n">
-        <v>2500</v>
+        <v>3970</v>
       </c>
       <c r="H62" t="n">
         <v>2500</v>
       </c>
       <c r="I62" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J62" t="n">
         <v>1750.849999999999</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>41.19</v>
       </c>
     </row>
@@ -2115,22 +2231,25 @@
         <v>4038.35</v>
       </c>
       <c r="D63" t="n">
-        <v>3000</v>
+        <v>3800</v>
       </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="n">
-        <v>3520</v>
+        <v>3510</v>
       </c>
       <c r="G63" t="n">
-        <v>2500</v>
+        <v>3670</v>
       </c>
       <c r="H63" t="n">
         <v>2500</v>
       </c>
       <c r="I63" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J63" t="n">
         <v>1538.35</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>38.09</v>
       </c>
     </row>
@@ -2145,22 +2264,25 @@
         <v>3825.85</v>
       </c>
       <c r="D64" t="n">
-        <v>2600</v>
+        <v>3200</v>
       </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="n">
-        <v>3330</v>
+        <v>3510</v>
       </c>
       <c r="G64" t="n">
-        <v>2400</v>
+        <v>3370</v>
       </c>
       <c r="H64" t="n">
         <v>2400</v>
       </c>
       <c r="I64" t="n">
+        <v>2400</v>
+      </c>
+      <c r="J64" t="n">
         <v>1425.85</v>
       </c>
-      <c r="J64" t="n">
+      <c r="K64" t="n">
         <v>37.27</v>
       </c>
     </row>
@@ -2175,22 +2297,25 @@
         <v>3400.85</v>
       </c>
       <c r="D65" t="n">
-        <v>2600</v>
+        <v>3200</v>
       </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="n">
-        <v>3330</v>
+        <v>3510</v>
       </c>
       <c r="G65" t="n">
-        <v>2400</v>
+        <v>3370</v>
       </c>
       <c r="H65" t="n">
         <v>2400</v>
       </c>
       <c r="I65" t="n">
+        <v>2400</v>
+      </c>
+      <c r="J65" t="n">
         <v>1000.85</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>29.43</v>
       </c>
     </row>
@@ -2205,22 +2330,25 @@
         <v>2975.85</v>
       </c>
       <c r="D66" t="n">
-        <v>2600</v>
+        <v>3200</v>
       </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="n">
-        <v>3254.76</v>
+        <v>3320</v>
       </c>
       <c r="G66" t="n">
-        <v>1900</v>
+        <v>3170</v>
       </c>
       <c r="H66" t="n">
         <v>1900</v>
       </c>
       <c r="I66" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J66" t="n">
         <v>1075.85</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>36.15</v>
       </c>
     </row>
@@ -2235,22 +2363,25 @@
         <v>2975.85</v>
       </c>
       <c r="D67" t="n">
-        <v>2100</v>
+        <v>2800</v>
       </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="n">
-        <v>3553.33</v>
+        <v>3320</v>
       </c>
       <c r="G67" t="n">
-        <v>1900</v>
+        <v>3170</v>
       </c>
       <c r="H67" t="n">
         <v>1900</v>
       </c>
       <c r="I67" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J67" t="n">
         <v>1075.85</v>
       </c>
-      <c r="J67" t="n">
+      <c r="K67" t="n">
         <v>36.15</v>
       </c>
     </row>
@@ -2272,13 +2403,14 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
-      <c r="H68" t="n">
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="n">
         <v>4722.599999999999</v>
       </c>
-      <c r="I68" t="n">
-        <v>0</v>
-      </c>
       <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2296,13 +2428,14 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
-      <c r="H69" t="n">
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="n">
         <v>4487.15</v>
       </c>
-      <c r="I69" t="n">
-        <v>0</v>
-      </c>
       <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2320,13 +2453,14 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
-      <c r="H70" t="n">
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="n">
         <v>4250.849999999999</v>
       </c>
-      <c r="I70" t="n">
-        <v>0</v>
-      </c>
       <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2344,13 +2478,14 @@
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
-      <c r="H71" t="n">
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="n">
         <v>3778.25</v>
       </c>
-      <c r="I71" t="n">
-        <v>0</v>
-      </c>
       <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2368,13 +2503,14 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
-      <c r="H72" t="n">
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="n">
         <v>3306.5</v>
       </c>
-      <c r="I72" t="n">
-        <v>0</v>
-      </c>
       <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2392,13 +2528,14 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
-      <c r="H73" t="n">
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="n">
         <v>3306.5</v>
       </c>
-      <c r="I73" t="n">
-        <v>0</v>
-      </c>
       <c r="J73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2422,15 +2559,18 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="n">
-        <v>2200</v>
+        <v>2970</v>
       </c>
       <c r="H74" t="n">
         <v>2200</v>
       </c>
       <c r="I74" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J74" t="n">
         <v>1233.15</v>
       </c>
-      <c r="J74" t="n">
+      <c r="K74" t="n">
         <v>35.92</v>
       </c>
     </row>
@@ -2450,15 +2590,18 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="n">
-        <v>2200</v>
+        <v>2770</v>
       </c>
       <c r="H75" t="n">
         <v>2200</v>
       </c>
       <c r="I75" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J75" t="n">
         <v>1062.3</v>
       </c>
-      <c r="J75" t="n">
+      <c r="K75" t="n">
         <v>32.56</v>
       </c>
     </row>
@@ -2478,15 +2621,18 @@
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="n">
-        <v>1900</v>
+        <v>2570</v>
       </c>
       <c r="H76" t="n">
         <v>1900</v>
       </c>
       <c r="I76" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J76" t="n">
         <v>1190.6</v>
       </c>
-      <c r="J76" t="n">
+      <c r="K76" t="n">
         <v>38.52</v>
       </c>
     </row>
@@ -2506,15 +2652,18 @@
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="n">
-        <v>1900</v>
+        <v>2570</v>
       </c>
       <c r="H77" t="n">
         <v>1900</v>
       </c>
       <c r="I77" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J77" t="n">
         <v>847.1999999999998</v>
       </c>
-      <c r="J77" t="n">
+      <c r="K77" t="n">
         <v>30.84</v>
       </c>
     </row>
@@ -2534,15 +2683,18 @@
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="n">
-        <v>1600</v>
+        <v>2470</v>
       </c>
       <c r="H78" t="n">
         <v>1600</v>
       </c>
       <c r="I78" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J78" t="n">
         <v>975.5</v>
       </c>
-      <c r="J78" t="n">
+      <c r="K78" t="n">
         <v>37.88</v>
       </c>
     </row>
@@ -2562,15 +2714,18 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="n">
-        <v>1600</v>
+        <v>2470</v>
       </c>
       <c r="H79" t="n">
         <v>1600</v>
       </c>
       <c r="I79" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J79" t="n">
         <v>803.7999999999997</v>
       </c>
-      <c r="J79" t="n">
+      <c r="K79" t="n">
         <v>33.44</v>
       </c>
     </row>
@@ -2589,17 +2744,22 @@
         <v>3813.95</v>
       </c>
       <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>4200</v>
+      </c>
       <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr"/>
-      <c r="H80" t="n">
-        <v>3813.95</v>
-      </c>
+      <c r="G80" t="n">
+        <v>3670</v>
+      </c>
+      <c r="H80" t="inlineStr"/>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>3670</v>
       </c>
       <c r="J80" t="n">
-        <v>0</v>
+        <v>143.9499999999998</v>
+      </c>
+      <c r="K80" t="n">
+        <v>3.77</v>
       </c>
     </row>
     <row r="81">
@@ -2613,17 +2773,22 @@
         <v>3623.55</v>
       </c>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>3866.67</v>
+      </c>
       <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
-      <c r="H81" t="n">
-        <v>3623.55</v>
-      </c>
+      <c r="G81" t="n">
+        <v>3470</v>
+      </c>
+      <c r="H81" t="inlineStr"/>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>3470</v>
       </c>
       <c r="J81" t="n">
-        <v>0</v>
+        <v>153.5499999999997</v>
+      </c>
+      <c r="K81" t="n">
+        <v>4.24</v>
       </c>
     </row>
     <row r="82">
@@ -2637,17 +2802,22 @@
         <v>3433.15</v>
       </c>
       <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>2871.43</v>
+      </c>
       <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr"/>
-      <c r="H82" t="n">
-        <v>3433.15</v>
-      </c>
+      <c r="G82" t="n">
+        <v>3170</v>
+      </c>
+      <c r="H82" t="inlineStr"/>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>2871.43</v>
       </c>
       <c r="J82" t="n">
-        <v>0</v>
+        <v>561.7200000000003</v>
+      </c>
+      <c r="K82" t="n">
+        <v>16.36</v>
       </c>
     </row>
     <row r="83">
@@ -2661,17 +2831,22 @@
         <v>3051.5</v>
       </c>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="n">
+        <v>2835.71</v>
+      </c>
       <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr"/>
-      <c r="H83" t="n">
-        <v>3051.5</v>
-      </c>
+      <c r="G83" t="n">
+        <v>3170</v>
+      </c>
+      <c r="H83" t="inlineStr"/>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>2835.71</v>
       </c>
       <c r="J83" t="n">
-        <v>0</v>
+        <v>215.79</v>
+      </c>
+      <c r="K83" t="n">
+        <v>7.07</v>
       </c>
     </row>
     <row r="84">
@@ -2685,17 +2860,22 @@
         <v>2861.1</v>
       </c>
       <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
+      <c r="E84" t="n">
+        <v>2823.81</v>
+      </c>
       <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr"/>
-      <c r="H84" t="n">
-        <v>2861.1</v>
-      </c>
+      <c r="G84" t="n">
+        <v>2970</v>
+      </c>
+      <c r="H84" t="inlineStr"/>
       <c r="I84" t="n">
-        <v>0</v>
+        <v>2823.81</v>
       </c>
       <c r="J84" t="n">
-        <v>0</v>
+        <v>37.28999999999996</v>
+      </c>
+      <c r="K84" t="n">
+        <v>1.3</v>
       </c>
     </row>
     <row r="85">
@@ -2709,16 +2889,21 @@
         <v>2669.85</v>
       </c>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>2816.67</v>
+      </c>
       <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="n">
+      <c r="G85" t="n">
+        <v>2970</v>
+      </c>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="n">
         <v>2669.85</v>
       </c>
-      <c r="I85" t="n">
-        <v>0</v>
-      </c>
       <c r="J85" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2740,13 +2925,14 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
-      <c r="H86" t="n">
-        <v>0</v>
-      </c>
+      <c r="H86" t="inlineStr"/>
       <c r="I86" t="n">
         <v>0</v>
       </c>
-      <c r="J86" t="inlineStr"/>
+      <c r="J86" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
@@ -2762,13 +2948,14 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
-      <c r="H87" t="n">
-        <v>0</v>
-      </c>
+      <c r="H87" t="inlineStr"/>
       <c r="I87" t="n">
         <v>0</v>
       </c>
-      <c r="J87" t="inlineStr"/>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
@@ -2784,13 +2971,14 @@
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
-      <c r="H88" t="n">
-        <v>0</v>
-      </c>
+      <c r="H88" t="inlineStr"/>
       <c r="I88" t="n">
         <v>0</v>
       </c>
-      <c r="J88" t="inlineStr"/>
+      <c r="J88" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
@@ -2806,13 +2994,14 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
-      <c r="H89" t="n">
-        <v>0</v>
-      </c>
+      <c r="H89" t="inlineStr"/>
       <c r="I89" t="n">
         <v>0</v>
       </c>
-      <c r="J89" t="inlineStr"/>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
@@ -2828,13 +3017,14 @@
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
-      <c r="H90" t="n">
-        <v>0</v>
-      </c>
+      <c r="H90" t="inlineStr"/>
       <c r="I90" t="n">
         <v>0</v>
       </c>
-      <c r="J90" t="inlineStr"/>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
@@ -2850,13 +3040,14 @@
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
-      <c r="H91" t="n">
-        <v>0</v>
-      </c>
+      <c r="H91" t="inlineStr"/>
       <c r="I91" t="n">
         <v>0</v>
       </c>
-      <c r="J91" t="inlineStr"/>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
@@ -2875,23 +3066,24 @@
       <c r="D92" t="n">
         <v>3700</v>
       </c>
-      <c r="E92" t="n">
-        <v>5200</v>
-      </c>
+      <c r="E92" t="inlineStr"/>
       <c r="F92" t="n">
+        <v>3770</v>
+      </c>
+      <c r="G92" t="n">
+        <v>3270</v>
+      </c>
+      <c r="H92" t="n">
         <v>3900</v>
       </c>
-      <c r="G92" t="n">
-        <v>3900</v>
-      </c>
-      <c r="H92" t="n">
-        <v>3700</v>
-      </c>
       <c r="I92" t="n">
-        <v>295.8499999999999</v>
+        <v>3270</v>
       </c>
       <c r="J92" t="n">
-        <v>7.4</v>
+        <v>725.8499999999999</v>
+      </c>
+      <c r="K92" t="n">
+        <v>18.17</v>
       </c>
     </row>
     <row r="93">
@@ -2907,23 +3099,24 @@
       <c r="D93" t="n">
         <v>3700</v>
       </c>
-      <c r="E93" t="n">
-        <v>4200</v>
-      </c>
+      <c r="E93" t="inlineStr"/>
       <c r="F93" t="n">
-        <v>3350</v>
+        <v>3250</v>
       </c>
       <c r="G93" t="n">
+        <v>3070</v>
+      </c>
+      <c r="H93" t="n">
         <v>3900</v>
       </c>
-      <c r="H93" t="n">
-        <v>3350</v>
-      </c>
       <c r="I93" t="n">
-        <v>446.0999999999999</v>
+        <v>3070</v>
       </c>
       <c r="J93" t="n">
-        <v>11.75</v>
+        <v>726.0999999999999</v>
+      </c>
+      <c r="K93" t="n">
+        <v>19.13</v>
       </c>
     </row>
     <row r="94">
@@ -2939,23 +3132,24 @@
       <c r="D94" t="n">
         <v>3200</v>
       </c>
-      <c r="E94" t="n">
-        <v>3014.29</v>
-      </c>
+      <c r="E94" t="inlineStr"/>
       <c r="F94" t="n">
-        <v>3250</v>
+        <v>3140</v>
       </c>
       <c r="G94" t="n">
+        <v>2870</v>
+      </c>
+      <c r="H94" t="n">
         <v>3500</v>
       </c>
-      <c r="H94" t="n">
-        <v>3014.29</v>
-      </c>
       <c r="I94" t="n">
-        <v>582.0599999999999</v>
+        <v>2870</v>
       </c>
       <c r="J94" t="n">
-        <v>16.18</v>
+        <v>726.3499999999999</v>
+      </c>
+      <c r="K94" t="n">
+        <v>20.2</v>
       </c>
     </row>
     <row r="95">
@@ -2971,23 +3165,24 @@
       <c r="D95" t="n">
         <v>3200</v>
       </c>
-      <c r="E95" t="n">
-        <v>2907.14</v>
-      </c>
+      <c r="E95" t="inlineStr"/>
       <c r="F95" t="n">
-        <v>3250</v>
+        <v>3140</v>
       </c>
       <c r="G95" t="n">
+        <v>2870</v>
+      </c>
+      <c r="H95" t="n">
         <v>3500</v>
       </c>
-      <c r="H95" t="n">
-        <v>2907.14</v>
-      </c>
       <c r="I95" t="n">
-        <v>289.71</v>
+        <v>2870</v>
       </c>
       <c r="J95" t="n">
-        <v>9.06</v>
+        <v>326.8499999999999</v>
+      </c>
+      <c r="K95" t="n">
+        <v>10.22</v>
       </c>
     </row>
     <row r="96">
@@ -3003,22 +3198,23 @@
       <c r="D96" t="n">
         <v>3200</v>
       </c>
-      <c r="E96" t="n">
-        <v>2871.43</v>
-      </c>
+      <c r="E96" t="inlineStr"/>
       <c r="F96" t="n">
-        <v>3164.76</v>
+        <v>3040</v>
       </c>
       <c r="G96" t="n">
-        <v>2500</v>
+        <v>2670</v>
       </c>
       <c r="H96" t="n">
         <v>2500</v>
       </c>
       <c r="I96" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J96" t="n">
         <v>297.3499999999999</v>
       </c>
-      <c r="J96" t="n">
+      <c r="K96" t="n">
         <v>10.63</v>
       </c>
     </row>
@@ -3035,22 +3231,23 @@
       <c r="D97" t="n">
         <v>2500</v>
       </c>
-      <c r="E97" t="n">
-        <v>2850</v>
-      </c>
+      <c r="E97" t="inlineStr"/>
       <c r="F97" t="n">
-        <v>3235.33</v>
+        <v>3040</v>
       </c>
       <c r="G97" t="n">
-        <v>2500</v>
+        <v>2670</v>
       </c>
       <c r="H97" t="n">
         <v>2500</v>
       </c>
       <c r="I97" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J97" t="n">
         <v>297.3499999999999</v>
       </c>
-      <c r="J97" t="n">
+      <c r="K97" t="n">
         <v>10.63</v>
       </c>
     </row>
@@ -3066,19 +3263,20 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>5333.75</v>
+        <v>4392.5</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr"/>
-      <c r="H98" t="n">
-        <v>5333.75</v>
-      </c>
+      <c r="H98" t="inlineStr"/>
       <c r="I98" t="n">
-        <v>0</v>
+        <v>4392.5</v>
       </c>
       <c r="J98" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3090,19 +3288,20 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>5067.7</v>
+        <v>4173.4</v>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr"/>
-      <c r="H99" t="n">
-        <v>5067.7</v>
-      </c>
+      <c r="H99" t="inlineStr"/>
       <c r="I99" t="n">
-        <v>0</v>
+        <v>4173.4</v>
       </c>
       <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3114,19 +3313,20 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4800.8</v>
+        <v>3953.6</v>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
-      <c r="H100" t="n">
-        <v>4800.8</v>
-      </c>
+      <c r="H100" t="inlineStr"/>
       <c r="I100" t="n">
-        <v>0</v>
+        <v>3953.6</v>
       </c>
       <c r="J100" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3138,19 +3338,20 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>4267</v>
+        <v>3514</v>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
-      <c r="H101" t="n">
-        <v>4267</v>
-      </c>
+      <c r="H101" t="inlineStr"/>
       <c r="I101" t="n">
-        <v>0</v>
+        <v>3514</v>
       </c>
       <c r="J101" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3162,19 +3363,20 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>3734.05</v>
+        <v>3075.099999999999</v>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
-      <c r="H102" t="n">
-        <v>3734.05</v>
-      </c>
+      <c r="H102" t="inlineStr"/>
       <c r="I102" t="n">
-        <v>0</v>
+        <v>3075.099999999999</v>
       </c>
       <c r="J102" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3186,19 +3388,20 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>3734.05</v>
+        <v>3075.099999999999</v>
       </c>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
-      <c r="H103" t="n">
-        <v>3734.05</v>
-      </c>
+      <c r="H103" t="inlineStr"/>
       <c r="I103" t="n">
-        <v>0</v>
+        <v>3075.099999999999</v>
       </c>
       <c r="J103" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3219,21 +3422,26 @@
       <c r="D104" t="n">
         <v>3700</v>
       </c>
-      <c r="E104" t="inlineStr"/>
+      <c r="E104" t="n">
+        <v>4200</v>
+      </c>
       <c r="F104" t="n">
-        <v>2950</v>
+        <v>2500</v>
       </c>
       <c r="G104" t="n">
-        <v>4000</v>
+        <v>3970</v>
       </c>
       <c r="H104" t="n">
-        <v>2950</v>
+        <v>3500</v>
       </c>
       <c r="I104" t="n">
-        <v>1442.5</v>
+        <v>2500</v>
       </c>
       <c r="J104" t="n">
-        <v>32.84</v>
+        <v>1892.5</v>
+      </c>
+      <c r="K104" t="n">
+        <v>43.08</v>
       </c>
     </row>
     <row r="105">
@@ -3249,21 +3457,26 @@
       <c r="D105" t="n">
         <v>3700</v>
       </c>
-      <c r="E105" t="inlineStr"/>
+      <c r="E105" t="n">
+        <v>3866.67</v>
+      </c>
       <c r="F105" t="n">
-        <v>2950</v>
+        <v>2500</v>
       </c>
       <c r="G105" t="n">
-        <v>4000</v>
+        <v>3770</v>
       </c>
       <c r="H105" t="n">
-        <v>2950</v>
+        <v>3500</v>
       </c>
       <c r="I105" t="n">
-        <v>1223.4</v>
+        <v>2500</v>
       </c>
       <c r="J105" t="n">
-        <v>29.31</v>
+        <v>1673.4</v>
+      </c>
+      <c r="K105" t="n">
+        <v>40.1</v>
       </c>
     </row>
     <row r="106">
@@ -3279,21 +3492,26 @@
       <c r="D106" t="n">
         <v>3300</v>
       </c>
-      <c r="E106" t="inlineStr"/>
+      <c r="E106" t="n">
+        <v>2871.43</v>
+      </c>
       <c r="F106" t="n">
-        <v>2780</v>
+        <v>2500</v>
       </c>
       <c r="G106" t="n">
-        <v>3800</v>
+        <v>3470</v>
       </c>
       <c r="H106" t="n">
-        <v>2780</v>
+        <v>3300</v>
       </c>
       <c r="I106" t="n">
-        <v>1173.6</v>
+        <v>2500</v>
       </c>
       <c r="J106" t="n">
-        <v>29.68</v>
+        <v>1453.6</v>
+      </c>
+      <c r="K106" t="n">
+        <v>36.77</v>
       </c>
     </row>
     <row r="107">
@@ -3309,21 +3527,26 @@
       <c r="D107" t="n">
         <v>3300</v>
       </c>
-      <c r="E107" t="inlineStr"/>
+      <c r="E107" t="n">
+        <v>2835.71</v>
+      </c>
       <c r="F107" t="n">
-        <v>2780</v>
+        <v>2500</v>
       </c>
       <c r="G107" t="n">
-        <v>3800</v>
+        <v>3470</v>
       </c>
       <c r="H107" t="n">
-        <v>2780</v>
+        <v>3300</v>
       </c>
       <c r="I107" t="n">
-        <v>734</v>
+        <v>2500</v>
       </c>
       <c r="J107" t="n">
-        <v>20.89</v>
+        <v>1014</v>
+      </c>
+      <c r="K107" t="n">
+        <v>28.86</v>
       </c>
     </row>
     <row r="108">
@@ -3339,20 +3562,25 @@
       <c r="D108" t="n">
         <v>3300</v>
       </c>
-      <c r="E108" t="inlineStr"/>
+      <c r="E108" t="n">
+        <v>2823.81</v>
+      </c>
       <c r="F108" t="n">
-        <v>2652.38</v>
+        <v>2500</v>
       </c>
       <c r="G108" t="n">
-        <v>2500</v>
+        <v>3270</v>
       </c>
       <c r="H108" t="n">
         <v>2500</v>
       </c>
       <c r="I108" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J108" t="n">
         <v>575.0999999999995</v>
       </c>
-      <c r="J108" t="n">
+      <c r="K108" t="n">
         <v>18.7</v>
       </c>
     </row>
@@ -3369,20 +3597,25 @@
       <c r="D109" t="n">
         <v>2800</v>
       </c>
-      <c r="E109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>2816.67</v>
+      </c>
       <c r="F109" t="n">
-        <v>2744.67</v>
+        <v>2500</v>
       </c>
       <c r="G109" t="n">
-        <v>2500</v>
+        <v>3270</v>
       </c>
       <c r="H109" t="n">
         <v>2500</v>
       </c>
       <c r="I109" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J109" t="n">
         <v>575.0999999999995</v>
       </c>
-      <c r="J109" t="n">
+      <c r="K109" t="n">
         <v>18.7</v>
       </c>
     </row>
@@ -3404,13 +3637,14 @@
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
-      <c r="H110" t="n">
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="n">
         <v>6361.4</v>
       </c>
-      <c r="I110" t="n">
-        <v>0</v>
-      </c>
       <c r="J110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K110" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3428,13 +3662,14 @@
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
-      <c r="H111" t="n">
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="n">
         <v>6043.5</v>
       </c>
-      <c r="I111" t="n">
-        <v>0</v>
-      </c>
       <c r="J111" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3452,13 +3687,14 @@
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
-      <c r="H112" t="n">
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="n">
         <v>5725.599999999999</v>
       </c>
-      <c r="I112" t="n">
-        <v>0</v>
-      </c>
       <c r="J112" t="n">
+        <v>0</v>
+      </c>
+      <c r="K112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3476,13 +3712,14 @@
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
-      <c r="H113" t="n">
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="n">
         <v>5089.8</v>
       </c>
-      <c r="I113" t="n">
-        <v>0</v>
-      </c>
       <c r="J113" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3500,13 +3737,14 @@
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
-      <c r="H114" t="n">
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="n">
         <v>4453.15</v>
       </c>
-      <c r="I114" t="n">
-        <v>0</v>
-      </c>
       <c r="J114" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3524,13 +3762,14 @@
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
-      <c r="H115" t="n">
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="n">
         <v>4453.15</v>
       </c>
-      <c r="I115" t="n">
-        <v>0</v>
-      </c>
       <c r="J115" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3549,25 +3788,28 @@
         <v>6361.4</v>
       </c>
       <c r="D116" t="n">
-        <v>3800</v>
+        <v>4500</v>
       </c>
       <c r="E116" t="n">
-        <v>10290</v>
+        <v>6308</v>
       </c>
       <c r="F116" t="n">
-        <v>2750</v>
+        <v>3470</v>
       </c>
       <c r="G116" t="n">
-        <v>3500</v>
+        <v>4770</v>
       </c>
       <c r="H116" t="n">
-        <v>2750</v>
+        <v>3900</v>
       </c>
       <c r="I116" t="n">
-        <v>3611.4</v>
+        <v>3470</v>
       </c>
       <c r="J116" t="n">
-        <v>56.77</v>
+        <v>2891.4</v>
+      </c>
+      <c r="K116" t="n">
+        <v>45.45</v>
       </c>
     </row>
     <row r="117">
@@ -3581,25 +3823,28 @@
         <v>6043.5</v>
       </c>
       <c r="D117" t="n">
-        <v>3800</v>
+        <v>4500</v>
       </c>
       <c r="E117" t="n">
-        <v>8096.67</v>
+        <v>5974.33</v>
       </c>
       <c r="F117" t="n">
-        <v>2750</v>
+        <v>3470</v>
       </c>
       <c r="G117" t="n">
-        <v>3500</v>
+        <v>4470</v>
       </c>
       <c r="H117" t="n">
-        <v>2750</v>
+        <v>3900</v>
       </c>
       <c r="I117" t="n">
-        <v>3293.5</v>
+        <v>3470</v>
       </c>
       <c r="J117" t="n">
-        <v>54.5</v>
+        <v>2573.5</v>
+      </c>
+      <c r="K117" t="n">
+        <v>42.58</v>
       </c>
     </row>
     <row r="118">
@@ -3613,25 +3858,28 @@
         <v>5725.599999999999</v>
       </c>
       <c r="D118" t="n">
-        <v>3350</v>
+        <v>4100</v>
       </c>
       <c r="E118" t="n">
-        <v>5601.29</v>
+        <v>5304</v>
       </c>
       <c r="F118" t="n">
-        <v>2750</v>
+        <v>3470</v>
       </c>
       <c r="G118" t="n">
-        <v>3300</v>
+        <v>4170</v>
       </c>
       <c r="H118" t="n">
-        <v>2750</v>
+        <v>3700</v>
       </c>
       <c r="I118" t="n">
-        <v>2975.599999999999</v>
+        <v>3470</v>
       </c>
       <c r="J118" t="n">
-        <v>51.97</v>
+        <v>2255.599999999999</v>
+      </c>
+      <c r="K118" t="n">
+        <v>39.39</v>
       </c>
     </row>
     <row r="119">
@@ -3645,25 +3893,28 @@
         <v>5089.8</v>
       </c>
       <c r="D119" t="n">
-        <v>3350</v>
+        <v>4100</v>
       </c>
       <c r="E119" t="n">
-        <v>5565.43</v>
+        <v>5268.21</v>
       </c>
       <c r="F119" t="n">
-        <v>2750</v>
+        <v>3470</v>
       </c>
       <c r="G119" t="n">
-        <v>3300</v>
+        <v>4170</v>
       </c>
       <c r="H119" t="n">
-        <v>2750</v>
+        <v>3700</v>
       </c>
       <c r="I119" t="n">
-        <v>2339.8</v>
+        <v>3470</v>
       </c>
       <c r="J119" t="n">
-        <v>45.97</v>
+        <v>1619.8</v>
+      </c>
+      <c r="K119" t="n">
+        <v>31.82</v>
       </c>
     </row>
     <row r="120">
@@ -3677,25 +3928,28 @@
         <v>4453.15</v>
       </c>
       <c r="D120" t="n">
-        <v>3350</v>
+        <v>4100</v>
       </c>
       <c r="E120" t="n">
-        <v>5359.14</v>
+        <v>5256.33</v>
       </c>
       <c r="F120" t="n">
-        <v>2648.1</v>
+        <v>3260</v>
       </c>
       <c r="G120" t="n">
-        <v>2500</v>
+        <v>3870</v>
       </c>
       <c r="H120" t="n">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="I120" t="n">
-        <v>1953.15</v>
+        <v>2700</v>
       </c>
       <c r="J120" t="n">
-        <v>43.86</v>
+        <v>1753.15</v>
+      </c>
+      <c r="K120" t="n">
+        <v>39.37</v>
       </c>
     </row>
     <row r="121">
@@ -3709,25 +3963,28 @@
         <v>4453.15</v>
       </c>
       <c r="D121" t="n">
-        <v>2900</v>
+        <v>3700</v>
       </c>
       <c r="E121" t="n">
-        <v>4900.53</v>
+        <v>4674.17</v>
       </c>
       <c r="F121" t="n">
-        <v>2813.67</v>
+        <v>3260</v>
       </c>
       <c r="G121" t="n">
-        <v>2500</v>
+        <v>3870</v>
       </c>
       <c r="H121" t="n">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="I121" t="n">
-        <v>1953.15</v>
+        <v>2700</v>
       </c>
       <c r="J121" t="n">
-        <v>43.86</v>
+        <v>1753.15</v>
+      </c>
+      <c r="K121" t="n">
+        <v>39.37</v>
       </c>
     </row>
     <row r="122">
@@ -3748,19 +4005,22 @@
         <v>9000</v>
       </c>
       <c r="E122" t="n">
-        <v>15020</v>
+        <v>11000</v>
       </c>
       <c r="F122" t="n">
         <v>8080</v>
       </c>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="n">
+      <c r="G122" t="n">
+        <v>8670</v>
+      </c>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="n">
         <v>5788.5</v>
       </c>
-      <c r="I122" t="n">
-        <v>0</v>
-      </c>
       <c r="J122" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3778,19 +4038,22 @@
         <v>9000</v>
       </c>
       <c r="E123" t="n">
-        <v>11928</v>
+        <v>9833.33</v>
       </c>
       <c r="F123" t="n">
         <v>7390</v>
       </c>
-      <c r="G123" t="inlineStr"/>
-      <c r="H123" t="n">
+      <c r="G123" t="n">
+        <v>8170</v>
+      </c>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="n">
         <v>5499.5</v>
       </c>
-      <c r="I123" t="n">
-        <v>0</v>
-      </c>
       <c r="J123" t="n">
+        <v>0</v>
+      </c>
+      <c r="K123" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3808,19 +4071,22 @@
         <v>8500</v>
       </c>
       <c r="E124" t="n">
-        <v>8268.57</v>
+        <v>7971.43</v>
       </c>
       <c r="F124" t="n">
         <v>6930</v>
       </c>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="n">
+      <c r="G124" t="n">
+        <v>7470</v>
+      </c>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="n">
         <v>5209.65</v>
       </c>
-      <c r="I124" t="n">
-        <v>0</v>
-      </c>
       <c r="J124" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3838,19 +4104,22 @@
         <v>8500</v>
       </c>
       <c r="E125" t="n">
-        <v>8232.93</v>
+        <v>6835.71</v>
       </c>
       <c r="F125" t="n">
         <v>6930</v>
       </c>
-      <c r="G125" t="inlineStr"/>
-      <c r="H125" t="n">
+      <c r="G125" t="n">
+        <v>7470</v>
+      </c>
+      <c r="H125" t="inlineStr"/>
+      <c r="I125" t="n">
         <v>4630.8</v>
       </c>
-      <c r="I125" t="n">
-        <v>0</v>
-      </c>
       <c r="J125" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3868,19 +4137,22 @@
         <v>8500</v>
       </c>
       <c r="E126" t="n">
-        <v>7799.81</v>
+        <v>6423.81</v>
       </c>
       <c r="F126" t="n">
         <v>6460</v>
       </c>
-      <c r="G126" t="inlineStr"/>
-      <c r="H126" t="n">
+      <c r="G126" t="n">
+        <v>6970</v>
+      </c>
+      <c r="H126" t="inlineStr"/>
+      <c r="I126" t="n">
         <v>4051.95</v>
       </c>
-      <c r="I126" t="n">
-        <v>0</v>
-      </c>
       <c r="J126" t="n">
+        <v>0</v>
+      </c>
+      <c r="K126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3898,19 +4170,22 @@
         <v>7500</v>
       </c>
       <c r="E127" t="n">
-        <v>7403.87</v>
+        <v>6016.67</v>
       </c>
       <c r="F127" t="n">
         <v>6460</v>
       </c>
-      <c r="G127" t="inlineStr"/>
-      <c r="H127" t="n">
+      <c r="G127" t="n">
+        <v>6970</v>
+      </c>
+      <c r="H127" t="inlineStr"/>
+      <c r="I127" t="n">
         <v>4051.95</v>
       </c>
-      <c r="I127" t="n">
-        <v>0</v>
-      </c>
       <c r="J127" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3932,13 +4207,14 @@
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
       <c r="G128" t="inlineStr"/>
-      <c r="H128" t="n">
+      <c r="H128" t="inlineStr"/>
+      <c r="I128" t="n">
         <v>7235.2</v>
       </c>
-      <c r="I128" t="n">
-        <v>0</v>
-      </c>
       <c r="J128" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3956,13 +4232,14 @@
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
-      <c r="H129" t="n">
+      <c r="H129" t="inlineStr"/>
+      <c r="I129" t="n">
         <v>6873.95</v>
       </c>
-      <c r="I129" t="n">
-        <v>0</v>
-      </c>
       <c r="J129" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3980,13 +4257,14 @@
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
-      <c r="H130" t="n">
+      <c r="H130" t="inlineStr"/>
+      <c r="I130" t="n">
         <v>6511.849999999999</v>
       </c>
-      <c r="I130" t="n">
-        <v>0</v>
-      </c>
       <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4004,13 +4282,14 @@
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
-      <c r="H131" t="n">
+      <c r="H131" t="inlineStr"/>
+      <c r="I131" t="n">
         <v>5788.5</v>
       </c>
-      <c r="I131" t="n">
-        <v>0</v>
-      </c>
       <c r="J131" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4028,13 +4307,14 @@
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
-      <c r="H132" t="n">
+      <c r="H132" t="inlineStr"/>
+      <c r="I132" t="n">
         <v>5065.15</v>
       </c>
-      <c r="I132" t="n">
-        <v>0</v>
-      </c>
       <c r="J132" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4052,13 +4332,14 @@
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
-      <c r="H133" t="n">
+      <c r="H133" t="inlineStr"/>
+      <c r="I133" t="n">
         <v>5065.15</v>
       </c>
-      <c r="I133" t="n">
-        <v>0</v>
-      </c>
       <c r="J133" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2 step - car_names added
</commit_message>
<xml_diff>
--- a/outputs/analysiss.xlsx
+++ b/outputs/analysiss.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K155"/>
+  <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,11 +505,6 @@
           <t>DELTA</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>DELTA %</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -522,15 +517,22 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Volkswagen Polo V</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Renault Logan</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
@@ -549,15 +551,8 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>1750</v>
-      </c>
-      <c r="J3" t="n">
-        <v>488.9000000000001</v>
-      </c>
-      <c r="K3" t="n">
-        <v>21.84</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
@@ -576,15 +571,8 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>1750</v>
-      </c>
-      <c r="J4" t="n">
-        <v>377.5499999999997</v>
-      </c>
-      <c r="K4" t="n">
-        <v>17.75</v>
-      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
@@ -603,15 +591,8 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J5" t="n">
-        <v>515.3499999999999</v>
-      </c>
-      <c r="K5" t="n">
-        <v>25.57</v>
-      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -630,15 +611,8 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J6" t="n">
-        <v>358.95</v>
-      </c>
-      <c r="K6" t="n">
-        <v>19.31</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
@@ -657,15 +631,8 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J7" t="n">
-        <v>246.75</v>
-      </c>
-      <c r="K7" t="n">
-        <v>14.13</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
@@ -684,15 +651,8 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>1450</v>
-      </c>
-      <c r="J8" t="n">
-        <v>229.5999999999999</v>
-      </c>
-      <c r="K8" t="n">
-        <v>13.67</v>
-      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -713,7 +673,6 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
@@ -730,15 +689,8 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
-        <v>2798.2</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -755,15 +707,8 @@
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>2658.8</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -780,15 +725,8 @@
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
-        <v>2518.55</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
@@ -805,15 +743,8 @@
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>2323.05</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
@@ -830,15 +761,8 @@
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
-        <v>2182.8</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
@@ -855,15 +779,8 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
-        <v>2098.65</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -884,7 +801,6 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
@@ -901,13 +817,8 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
@@ -924,13 +835,8 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
@@ -947,13 +853,8 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
@@ -970,13 +871,8 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
@@ -993,13 +889,8 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
@@ -1016,13 +907,8 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -1035,15 +921,22 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Lada Largus II</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Lada Largus 7 мест MT</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -1062,15 +955,8 @@
         <v>3470</v>
       </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
-        <v>3280.15</v>
-      </c>
-      <c r="J24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
@@ -1089,15 +975,8 @@
         <v>3270</v>
       </c>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
-        <v>3116.95</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
@@ -1116,15 +995,8 @@
         <v>2970</v>
       </c>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
-        <v>2952.9</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
@@ -1143,15 +1015,8 @@
         <v>2970</v>
       </c>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="n">
-        <v>2624.8</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0</v>
-      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
@@ -1170,15 +1035,8 @@
         <v>2870</v>
       </c>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="n">
-        <v>2296.7</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
@@ -1197,15 +1055,8 @@
         <v>2870</v>
       </c>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="n">
-        <v>2296.7</v>
-      </c>
-      <c r="J29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1218,7 +1069,11 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hyundai Solaris II</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -1226,7 +1081,6 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
@@ -1243,15 +1097,8 @@
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
-      <c r="I31" t="n">
-        <v>2431.85</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
@@ -1268,15 +1115,8 @@
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" t="n">
-        <v>2310.3</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
@@ -1293,15 +1133,8 @@
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="n">
-        <v>2188.75</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
@@ -1318,15 +1151,8 @@
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="n">
-        <v>2018.75</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
@@ -1343,15 +1169,8 @@
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" t="n">
-        <v>1897.2</v>
-      </c>
-      <c r="J35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
@@ -1368,15 +1187,8 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="n">
-        <v>1824.1</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1389,15 +1201,34 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hyundai Solaris II rest.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Hyundai Solaris</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Сhangan Alsvin / Renault Logan</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Hyundai Solaris II Promo</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Hyundai Solaris sedan</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
@@ -1422,15 +1253,8 @@
       <c r="H38" t="n">
         <v>2000</v>
       </c>
-      <c r="I38" t="n">
-        <v>2000</v>
-      </c>
-      <c r="J38" t="n">
-        <v>1039.6</v>
-      </c>
-      <c r="K38" t="n">
-        <v>34.2</v>
-      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
@@ -1455,15 +1279,8 @@
       <c r="H39" t="n">
         <v>2000</v>
       </c>
-      <c r="I39" t="n">
-        <v>2000</v>
-      </c>
-      <c r="J39" t="n">
-        <v>888.2999999999997</v>
-      </c>
-      <c r="K39" t="n">
-        <v>30.76</v>
-      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
@@ -1488,15 +1305,8 @@
       <c r="H40" t="n">
         <v>1800</v>
       </c>
-      <c r="I40" t="n">
-        <v>1800</v>
-      </c>
-      <c r="J40" t="n">
-        <v>936.1500000000001</v>
-      </c>
-      <c r="K40" t="n">
-        <v>34.21</v>
-      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
@@ -1521,15 +1331,8 @@
       <c r="H41" t="n">
         <v>1800</v>
       </c>
-      <c r="I41" t="n">
-        <v>1800</v>
-      </c>
-      <c r="J41" t="n">
-        <v>723.6500000000001</v>
-      </c>
-      <c r="K41" t="n">
-        <v>28.67</v>
-      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
@@ -1554,15 +1357,8 @@
       <c r="H42" t="n">
         <v>1500</v>
       </c>
-      <c r="I42" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J42" t="n">
-        <v>871.5</v>
-      </c>
-      <c r="K42" t="n">
-        <v>36.75</v>
-      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
@@ -1587,15 +1383,8 @@
       <c r="H43" t="n">
         <v>1500</v>
       </c>
-      <c r="I43" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J43" t="n">
-        <v>779.6999999999998</v>
-      </c>
-      <c r="K43" t="n">
-        <v>34.2</v>
-      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1608,7 +1397,11 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Skoda Rapid I rest.</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
@@ -1616,7 +1409,6 @@
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
@@ -1633,15 +1425,8 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
-      <c r="I45" t="n">
-        <v>2809.25</v>
-      </c>
-      <c r="J45" t="n">
-        <v>0</v>
-      </c>
-      <c r="K45" t="n">
-        <v>0</v>
-      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
@@ -1658,15 +1443,8 @@
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="n">
-        <v>2669</v>
-      </c>
-      <c r="J46" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
@@ -1683,15 +1461,8 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
-      <c r="I47" t="n">
-        <v>2528.75</v>
-      </c>
-      <c r="J47" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" t="n">
-        <v>0</v>
-      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
@@ -1708,15 +1479,8 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="n">
-        <v>2247.4</v>
-      </c>
-      <c r="J48" t="n">
-        <v>0</v>
-      </c>
-      <c r="K48" t="n">
-        <v>0</v>
-      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
@@ -1733,15 +1497,8 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
-      <c r="I49" t="n">
-        <v>1966.9</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0</v>
-      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
@@ -1758,15 +1515,8 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
-      <c r="I50" t="n">
-        <v>1966.9</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K50" t="n">
-        <v>0</v>
-      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1779,15 +1529,26 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Volkswagen Polo VI; Skoda Rapid II</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Volkswagen Polo АТ Promo</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skoda Rapid </t>
+        </is>
+      </c>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
-      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
@@ -1808,15 +1569,8 @@
       <c r="H52" t="n">
         <v>1800</v>
       </c>
-      <c r="I52" t="n">
-        <v>1800</v>
-      </c>
-      <c r="J52" t="n">
-        <v>1711.35</v>
-      </c>
-      <c r="K52" t="n">
-        <v>48.74</v>
-      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
@@ -1837,15 +1591,8 @@
       <c r="H53" t="n">
         <v>1800</v>
       </c>
-      <c r="I53" t="n">
-        <v>1800</v>
-      </c>
-      <c r="J53" t="n">
-        <v>1536.25</v>
-      </c>
-      <c r="K53" t="n">
-        <v>46.05</v>
-      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
@@ -1866,15 +1613,8 @@
       <c r="H54" t="n">
         <v>1600</v>
       </c>
-      <c r="I54" t="n">
-        <v>1600</v>
-      </c>
-      <c r="J54" t="n">
-        <v>1560.3</v>
-      </c>
-      <c r="K54" t="n">
-        <v>49.37</v>
-      </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
@@ -1895,15 +1635,8 @@
       <c r="H55" t="n">
         <v>1600</v>
       </c>
-      <c r="I55" t="n">
-        <v>1600</v>
-      </c>
-      <c r="J55" t="n">
-        <v>1209.25</v>
-      </c>
-      <c r="K55" t="n">
-        <v>43.05</v>
-      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
@@ -1924,15 +1657,8 @@
       <c r="H56" t="n">
         <v>1400</v>
       </c>
-      <c r="I56" t="n">
-        <v>1400</v>
-      </c>
-      <c r="J56" t="n">
-        <v>1058.2</v>
-      </c>
-      <c r="K56" t="n">
-        <v>43.05</v>
-      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
@@ -1953,15 +1679,8 @@
       <c r="H57" t="n">
         <v>1400</v>
       </c>
-      <c r="I57" t="n">
-        <v>1400</v>
-      </c>
-      <c r="J57" t="n">
-        <v>1058.2</v>
-      </c>
-      <c r="K57" t="n">
-        <v>43.05</v>
-      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1974,15 +1693,26 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Skoda Octavia A7 rest.; Hyundai Elantra VI rest.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Peugeot 408</t>
+        </is>
+      </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Nissan Almera</t>
+        </is>
+      </c>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
@@ -2003,15 +1733,8 @@
       <c r="H59" t="n">
         <v>1800</v>
       </c>
-      <c r="I59" t="n">
-        <v>1800</v>
-      </c>
-      <c r="J59" t="n">
-        <v>1336.5</v>
-      </c>
-      <c r="K59" t="n">
-        <v>42.61</v>
-      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
@@ -2032,15 +1755,8 @@
       <c r="H60" t="n">
         <v>1800</v>
       </c>
-      <c r="I60" t="n">
-        <v>1800</v>
-      </c>
-      <c r="J60" t="n">
-        <v>1180.1</v>
-      </c>
-      <c r="K60" t="n">
-        <v>39.6</v>
-      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
@@ -2061,15 +1777,8 @@
       <c r="H61" t="n">
         <v>1600</v>
       </c>
-      <c r="I61" t="n">
-        <v>1600</v>
-      </c>
-      <c r="J61" t="n">
-        <v>1222.85</v>
-      </c>
-      <c r="K61" t="n">
-        <v>43.32</v>
-      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
@@ -2090,15 +1799,8 @@
       <c r="H62" t="n">
         <v>1600</v>
       </c>
-      <c r="I62" t="n">
-        <v>1600</v>
-      </c>
-      <c r="J62" t="n">
-        <v>909.1999999999998</v>
-      </c>
-      <c r="K62" t="n">
-        <v>36.23</v>
-      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
@@ -2119,15 +1821,8 @@
       <c r="H63" t="n">
         <v>1200</v>
       </c>
-      <c r="I63" t="n">
-        <v>1200</v>
-      </c>
-      <c r="J63" t="n">
-        <v>995.5499999999997</v>
-      </c>
-      <c r="K63" t="n">
-        <v>45.34</v>
-      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
@@ -2148,15 +1843,8 @@
       <c r="H64" t="n">
         <v>1200</v>
       </c>
-      <c r="I64" t="n">
-        <v>1200</v>
-      </c>
-      <c r="J64" t="n">
-        <v>995.5499999999997</v>
-      </c>
-      <c r="K64" t="n">
-        <v>45.34</v>
-      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -2169,15 +1857,26 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyundai Elantra VII </t>
+        </is>
+      </c>
       <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Changan UNI-V</t>
+        </is>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Chevrolet Cruze sedan</t>
+        </is>
+      </c>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
-      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
@@ -2198,15 +1897,8 @@
       <c r="H66" t="n">
         <v>2100</v>
       </c>
-      <c r="I66" t="n">
-        <v>2100</v>
-      </c>
-      <c r="J66" t="n">
-        <v>1589.85</v>
-      </c>
-      <c r="K66" t="n">
-        <v>43.09</v>
-      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
@@ -2227,15 +1919,8 @@
       <c r="H67" t="n">
         <v>2100</v>
       </c>
-      <c r="I67" t="n">
-        <v>2100</v>
-      </c>
-      <c r="J67" t="n">
-        <v>1405.4</v>
-      </c>
-      <c r="K67" t="n">
-        <v>40.09</v>
-      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
@@ -2256,15 +1941,8 @@
       <c r="H68" t="n">
         <v>1900</v>
       </c>
-      <c r="I68" t="n">
-        <v>1900</v>
-      </c>
-      <c r="J68" t="n">
-        <v>1420.95</v>
-      </c>
-      <c r="K68" t="n">
-        <v>42.79</v>
-      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
@@ -2285,15 +1963,8 @@
       <c r="H69" t="n">
         <v>1900</v>
       </c>
-      <c r="I69" t="n">
-        <v>1900</v>
-      </c>
-      <c r="J69" t="n">
-        <v>1052.05</v>
-      </c>
-      <c r="K69" t="n">
-        <v>35.64</v>
-      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
@@ -2314,15 +1985,8 @@
       <c r="H70" t="n">
         <v>1500</v>
       </c>
-      <c r="I70" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J70" t="n">
-        <v>1083.15</v>
-      </c>
-      <c r="K70" t="n">
-        <v>41.93</v>
-      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
@@ -2343,15 +2007,8 @@
       <c r="H71" t="n">
         <v>1500</v>
       </c>
-      <c r="I71" t="n">
-        <v>1500</v>
-      </c>
-      <c r="J71" t="n">
-        <v>1083.15</v>
-      </c>
-      <c r="K71" t="n">
-        <v>41.93</v>
-      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -2364,15 +2021,34 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>KIA Optima IV rest.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Hyundai Sonata</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Hyundai Sonata VIII 2.5</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Hyundai Sonata AT Promo</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Hyundai i40</t>
+        </is>
+      </c>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
@@ -2397,15 +2073,8 @@
       <c r="H73" t="n">
         <v>2500</v>
       </c>
-      <c r="I73" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J73" t="n">
-        <v>1750.849999999999</v>
-      </c>
-      <c r="K73" t="n">
-        <v>41.19</v>
-      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
@@ -2430,15 +2099,8 @@
       <c r="H74" t="n">
         <v>2500</v>
       </c>
-      <c r="I74" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J74" t="n">
-        <v>1538.35</v>
-      </c>
-      <c r="K74" t="n">
-        <v>38.09</v>
-      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
@@ -2463,15 +2125,8 @@
       <c r="H75" t="n">
         <v>2400</v>
       </c>
-      <c r="I75" t="n">
-        <v>2400</v>
-      </c>
-      <c r="J75" t="n">
-        <v>1425.85</v>
-      </c>
-      <c r="K75" t="n">
-        <v>37.27</v>
-      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
@@ -2496,15 +2151,8 @@
       <c r="H76" t="n">
         <v>2400</v>
       </c>
-      <c r="I76" t="n">
-        <v>2400</v>
-      </c>
-      <c r="J76" t="n">
-        <v>1000.85</v>
-      </c>
-      <c r="K76" t="n">
-        <v>29.43</v>
-      </c>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
@@ -2529,15 +2177,8 @@
       <c r="H77" t="n">
         <v>1900</v>
       </c>
-      <c r="I77" t="n">
-        <v>1900</v>
-      </c>
-      <c r="J77" t="n">
-        <v>1075.85</v>
-      </c>
-      <c r="K77" t="n">
-        <v>36.15</v>
-      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
@@ -2562,15 +2203,8 @@
       <c r="H78" t="n">
         <v>1900</v>
       </c>
-      <c r="I78" t="n">
-        <v>1900</v>
-      </c>
-      <c r="J78" t="n">
-        <v>1075.85</v>
-      </c>
-      <c r="K78" t="n">
-        <v>36.15</v>
-      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -2591,7 +2225,6 @@
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
-      <c r="K79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
@@ -2608,15 +2241,8 @@
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="n">
-        <v>4722.599999999999</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0</v>
-      </c>
-      <c r="K80" t="n">
-        <v>0</v>
-      </c>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
@@ -2633,15 +2259,8 @@
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
-      <c r="I81" t="n">
-        <v>4487.15</v>
-      </c>
-      <c r="J81" t="n">
-        <v>0</v>
-      </c>
-      <c r="K81" t="n">
-        <v>0</v>
-      </c>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
@@ -2658,15 +2277,8 @@
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
-      <c r="I82" t="n">
-        <v>4250.849999999999</v>
-      </c>
-      <c r="J82" t="n">
-        <v>0</v>
-      </c>
-      <c r="K82" t="n">
-        <v>0</v>
-      </c>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
@@ -2683,15 +2295,8 @@
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
-      <c r="I83" t="n">
-        <v>3778.25</v>
-      </c>
-      <c r="J83" t="n">
-        <v>0</v>
-      </c>
-      <c r="K83" t="n">
-        <v>0</v>
-      </c>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
@@ -2708,15 +2313,8 @@
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
-      <c r="I84" t="n">
-        <v>3306.5</v>
-      </c>
-      <c r="J84" t="n">
-        <v>0</v>
-      </c>
-      <c r="K84" t="n">
-        <v>0</v>
-      </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
@@ -2733,15 +2331,8 @@
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
-      <c r="I85" t="n">
-        <v>3306.5</v>
-      </c>
-      <c r="J85" t="n">
-        <v>0</v>
-      </c>
-      <c r="K85" t="n">
-        <v>0</v>
-      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -2754,15 +2345,30 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Hyundai CRETA I</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Hyundai Creta</t>
+        </is>
+      </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Hyundai Creta AT Promo</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Renault Kaptur</t>
+        </is>
+      </c>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
@@ -2785,15 +2391,8 @@
       <c r="H87" t="n">
         <v>2200</v>
       </c>
-      <c r="I87" t="n">
-        <v>2200</v>
-      </c>
-      <c r="J87" t="n">
-        <v>1233.15</v>
-      </c>
-      <c r="K87" t="n">
-        <v>35.92</v>
-      </c>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
@@ -2816,15 +2415,8 @@
       <c r="H88" t="n">
         <v>2200</v>
       </c>
-      <c r="I88" t="n">
-        <v>2200</v>
-      </c>
-      <c r="J88" t="n">
-        <v>1062.3</v>
-      </c>
-      <c r="K88" t="n">
-        <v>32.56</v>
-      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
@@ -2847,15 +2439,8 @@
       <c r="H89" t="n">
         <v>1900</v>
       </c>
-      <c r="I89" t="n">
-        <v>1900</v>
-      </c>
-      <c r="J89" t="n">
-        <v>1190.6</v>
-      </c>
-      <c r="K89" t="n">
-        <v>38.52</v>
-      </c>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
@@ -2878,15 +2463,8 @@
       <c r="H90" t="n">
         <v>1900</v>
       </c>
-      <c r="I90" t="n">
-        <v>1900</v>
-      </c>
-      <c r="J90" t="n">
-        <v>847.1999999999998</v>
-      </c>
-      <c r="K90" t="n">
-        <v>30.84</v>
-      </c>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
@@ -2909,15 +2487,8 @@
       <c r="H91" t="n">
         <v>1600</v>
       </c>
-      <c r="I91" t="n">
-        <v>1600</v>
-      </c>
-      <c r="J91" t="n">
-        <v>975.5</v>
-      </c>
-      <c r="K91" t="n">
-        <v>37.88</v>
-      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
@@ -2940,15 +2511,8 @@
       <c r="H92" t="n">
         <v>1600</v>
       </c>
-      <c r="I92" t="n">
-        <v>1600</v>
-      </c>
-      <c r="J92" t="n">
-        <v>803.7999999999997</v>
-      </c>
-      <c r="K92" t="n">
-        <v>33.44</v>
-      </c>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -2961,15 +2525,26 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Hyundai CRETA I rest.</t>
+        </is>
+      </c>
       <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Сhery Tiggo 4</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Renault Duster 4WD AT</t>
+        </is>
+      </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
@@ -2990,15 +2565,8 @@
         <v>3670</v>
       </c>
       <c r="H94" t="inlineStr"/>
-      <c r="I94" t="n">
-        <v>3670</v>
-      </c>
-      <c r="J94" t="n">
-        <v>143.9499999999998</v>
-      </c>
-      <c r="K94" t="n">
-        <v>3.77</v>
-      </c>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
@@ -3019,15 +2587,8 @@
         <v>3470</v>
       </c>
       <c r="H95" t="inlineStr"/>
-      <c r="I95" t="n">
-        <v>3470</v>
-      </c>
-      <c r="J95" t="n">
-        <v>153.5499999999997</v>
-      </c>
-      <c r="K95" t="n">
-        <v>4.24</v>
-      </c>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
@@ -3048,15 +2609,8 @@
         <v>3170</v>
       </c>
       <c r="H96" t="inlineStr"/>
-      <c r="I96" t="n">
-        <v>2871.43</v>
-      </c>
-      <c r="J96" t="n">
-        <v>561.7200000000003</v>
-      </c>
-      <c r="K96" t="n">
-        <v>16.36</v>
-      </c>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
@@ -3077,15 +2631,8 @@
         <v>3170</v>
       </c>
       <c r="H97" t="inlineStr"/>
-      <c r="I97" t="n">
-        <v>2835.71</v>
-      </c>
-      <c r="J97" t="n">
-        <v>215.79</v>
-      </c>
-      <c r="K97" t="n">
-        <v>7.07</v>
-      </c>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
@@ -3106,15 +2653,8 @@
         <v>2970</v>
       </c>
       <c r="H98" t="inlineStr"/>
-      <c r="I98" t="n">
-        <v>2823.81</v>
-      </c>
-      <c r="J98" t="n">
-        <v>37.28999999999996</v>
-      </c>
-      <c r="K98" t="n">
-        <v>1.3</v>
-      </c>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
@@ -3135,15 +2675,8 @@
         <v>2970</v>
       </c>
       <c r="H99" t="inlineStr"/>
-      <c r="I99" t="n">
-        <v>2669.85</v>
-      </c>
-      <c r="J99" t="n">
-        <v>0</v>
-      </c>
-      <c r="K99" t="n">
-        <v>0</v>
-      </c>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
@@ -3164,7 +2697,6 @@
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
@@ -3181,13 +2713,8 @@
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
-      <c r="I101" t="n">
-        <v>0</v>
-      </c>
-      <c r="J101" t="n">
-        <v>0</v>
-      </c>
-      <c r="K101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
@@ -3204,13 +2731,8 @@
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
-      <c r="I102" t="n">
-        <v>0</v>
-      </c>
-      <c r="J102" t="n">
-        <v>0</v>
-      </c>
-      <c r="K102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
@@ -3227,13 +2749,8 @@
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
-      <c r="I103" t="n">
-        <v>0</v>
-      </c>
-      <c r="J103" t="n">
-        <v>0</v>
-      </c>
-      <c r="K103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
@@ -3250,13 +2767,8 @@
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
-      <c r="I104" t="n">
-        <v>0</v>
-      </c>
-      <c r="J104" t="n">
-        <v>0</v>
-      </c>
-      <c r="K104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
@@ -3273,13 +2785,8 @@
       <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
-      <c r="I105" t="n">
-        <v>0</v>
-      </c>
-      <c r="J105" t="n">
-        <v>0</v>
-      </c>
-      <c r="K105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n"/>
@@ -3296,13 +2803,8 @@
       <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
-      <c r="I106" t="n">
-        <v>0</v>
-      </c>
-      <c r="J106" t="n">
-        <v>0</v>
-      </c>
-      <c r="K106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
@@ -3315,15 +2817,35 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Geely COOLRAY I; Hyundai CRETA II; 
+Nissan Qashqai II rest.</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Hyundai Creta NEW</t>
+        </is>
+      </c>
       <c r="E107" t="inlineStr"/>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Geely Coolray</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Renault Kaptur AT Promo</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Toyota CH R</t>
+        </is>
+      </c>
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
@@ -3348,15 +2870,8 @@
       <c r="H108" t="n">
         <v>3900</v>
       </c>
-      <c r="I108" t="n">
-        <v>3270</v>
-      </c>
-      <c r="J108" t="n">
-        <v>725.8499999999999</v>
-      </c>
-      <c r="K108" t="n">
-        <v>18.17</v>
-      </c>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n"/>
@@ -3381,15 +2896,8 @@
       <c r="H109" t="n">
         <v>3900</v>
       </c>
-      <c r="I109" t="n">
-        <v>3070</v>
-      </c>
-      <c r="J109" t="n">
-        <v>726.0999999999999</v>
-      </c>
-      <c r="K109" t="n">
-        <v>19.13</v>
-      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n"/>
@@ -3414,15 +2922,8 @@
       <c r="H110" t="n">
         <v>3500</v>
       </c>
-      <c r="I110" t="n">
-        <v>2870</v>
-      </c>
-      <c r="J110" t="n">
-        <v>726.3499999999999</v>
-      </c>
-      <c r="K110" t="n">
-        <v>20.2</v>
-      </c>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
@@ -3447,15 +2948,8 @@
       <c r="H111" t="n">
         <v>3500</v>
       </c>
-      <c r="I111" t="n">
-        <v>2870</v>
-      </c>
-      <c r="J111" t="n">
-        <v>326.8499999999999</v>
-      </c>
-      <c r="K111" t="n">
-        <v>10.22</v>
-      </c>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n"/>
@@ -3480,15 +2974,8 @@
       <c r="H112" t="n">
         <v>2500</v>
       </c>
-      <c r="I112" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J112" t="n">
-        <v>297.3499999999999</v>
-      </c>
-      <c r="K112" t="n">
-        <v>10.63</v>
-      </c>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n"/>
@@ -3513,15 +3000,8 @@
       <c r="H113" t="n">
         <v>2500</v>
       </c>
-      <c r="I113" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J113" t="n">
-        <v>297.3499999999999</v>
-      </c>
-      <c r="K113" t="n">
-        <v>10.63</v>
-      </c>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
@@ -3542,7 +3022,6 @@
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
-      <c r="K114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n"/>
@@ -3551,23 +3030,14 @@
           <t>r1</t>
         </is>
       </c>
-      <c r="C115" t="n">
-        <v>4392.5</v>
-      </c>
+      <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
-      <c r="I115" t="n">
-        <v>4392.5</v>
-      </c>
-      <c r="J115" t="n">
-        <v>0</v>
-      </c>
-      <c r="K115" t="n">
-        <v>0</v>
-      </c>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n"/>
@@ -3576,23 +3046,14 @@
           <t>r3</t>
         </is>
       </c>
-      <c r="C116" t="n">
-        <v>4173.4</v>
-      </c>
+      <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="n">
-        <v>4173.4</v>
-      </c>
-      <c r="J116" t="n">
-        <v>0</v>
-      </c>
-      <c r="K116" t="n">
-        <v>0</v>
-      </c>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n"/>
@@ -3601,23 +3062,14 @@
           <t>r7</t>
         </is>
       </c>
-      <c r="C117" t="n">
-        <v>3953.6</v>
-      </c>
+      <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
-      <c r="I117" t="n">
-        <v>3953.6</v>
-      </c>
-      <c r="J117" t="n">
-        <v>0</v>
-      </c>
-      <c r="K117" t="n">
-        <v>0</v>
-      </c>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
@@ -3626,23 +3078,14 @@
           <t>r14</t>
         </is>
       </c>
-      <c r="C118" t="n">
-        <v>3514</v>
-      </c>
+      <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
-      <c r="I118" t="n">
-        <v>3514</v>
-      </c>
-      <c r="J118" t="n">
-        <v>0</v>
-      </c>
-      <c r="K118" t="n">
-        <v>0</v>
-      </c>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n"/>
@@ -3651,23 +3094,14 @@
           <t>r21</t>
         </is>
       </c>
-      <c r="C119" t="n">
-        <v>3075.099999999999</v>
-      </c>
+      <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
-      <c r="I119" t="n">
-        <v>3075.099999999999</v>
-      </c>
-      <c r="J119" t="n">
-        <v>0</v>
-      </c>
-      <c r="K119" t="n">
-        <v>0</v>
-      </c>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
@@ -3676,23 +3110,14 @@
           <t>r30</t>
         </is>
       </c>
-      <c r="C120" t="n">
-        <v>3075.099999999999</v>
-      </c>
+      <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
-      <c r="I120" t="n">
-        <v>3075.099999999999</v>
-      </c>
-      <c r="J120" t="n">
-        <v>0</v>
-      </c>
-      <c r="K120" t="n">
-        <v>0</v>
-      </c>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
@@ -3706,14 +3131,33 @@
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr"/>
-      <c r="E121" t="inlineStr"/>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
-      <c r="H121" t="inlineStr"/>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Haval Jolion</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Haval Jolion</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haval M6 </t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Haval Jolion AT</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Kia Sportage SLS</t>
+        </is>
+      </c>
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
-      <c r="K121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n"/>
@@ -3722,9 +3166,7 @@
           <t>r1</t>
         </is>
       </c>
-      <c r="C122" t="n">
-        <v>4392.5</v>
-      </c>
+      <c r="C122" t="inlineStr"/>
       <c r="D122" t="n">
         <v>3700</v>
       </c>
@@ -3740,15 +3182,8 @@
       <c r="H122" t="n">
         <v>3500</v>
       </c>
-      <c r="I122" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J122" t="n">
-        <v>1892.5</v>
-      </c>
-      <c r="K122" t="n">
-        <v>43.08</v>
-      </c>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n"/>
@@ -3757,9 +3192,7 @@
           <t>r3</t>
         </is>
       </c>
-      <c r="C123" t="n">
-        <v>4173.4</v>
-      </c>
+      <c r="C123" t="inlineStr"/>
       <c r="D123" t="n">
         <v>3700</v>
       </c>
@@ -3775,15 +3208,8 @@
       <c r="H123" t="n">
         <v>3500</v>
       </c>
-      <c r="I123" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J123" t="n">
-        <v>1673.4</v>
-      </c>
-      <c r="K123" t="n">
-        <v>40.1</v>
-      </c>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n"/>
@@ -3792,9 +3218,7 @@
           <t>r7</t>
         </is>
       </c>
-      <c r="C124" t="n">
-        <v>3953.6</v>
-      </c>
+      <c r="C124" t="inlineStr"/>
       <c r="D124" t="n">
         <v>3300</v>
       </c>
@@ -3810,15 +3234,8 @@
       <c r="H124" t="n">
         <v>3300</v>
       </c>
-      <c r="I124" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J124" t="n">
-        <v>1453.6</v>
-      </c>
-      <c r="K124" t="n">
-        <v>36.77</v>
-      </c>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n"/>
@@ -3827,9 +3244,7 @@
           <t>r14</t>
         </is>
       </c>
-      <c r="C125" t="n">
-        <v>3514</v>
-      </c>
+      <c r="C125" t="inlineStr"/>
       <c r="D125" t="n">
         <v>3300</v>
       </c>
@@ -3845,15 +3260,8 @@
       <c r="H125" t="n">
         <v>3300</v>
       </c>
-      <c r="I125" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J125" t="n">
-        <v>1014</v>
-      </c>
-      <c r="K125" t="n">
-        <v>28.86</v>
-      </c>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
@@ -3862,9 +3270,7 @@
           <t>r21</t>
         </is>
       </c>
-      <c r="C126" t="n">
-        <v>3075.099999999999</v>
-      </c>
+      <c r="C126" t="inlineStr"/>
       <c r="D126" t="n">
         <v>3300</v>
       </c>
@@ -3880,15 +3286,8 @@
       <c r="H126" t="n">
         <v>2500</v>
       </c>
-      <c r="I126" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J126" t="n">
-        <v>575.0999999999995</v>
-      </c>
-      <c r="K126" t="n">
-        <v>18.7</v>
-      </c>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n"/>
@@ -3897,9 +3296,7 @@
           <t>r30</t>
         </is>
       </c>
-      <c r="C127" t="n">
-        <v>3075.099999999999</v>
-      </c>
+      <c r="C127" t="inlineStr"/>
       <c r="D127" t="n">
         <v>2800</v>
       </c>
@@ -3915,15 +3312,8 @@
       <c r="H127" t="n">
         <v>2500</v>
       </c>
-      <c r="I127" t="n">
-        <v>2500</v>
-      </c>
-      <c r="J127" t="n">
-        <v>575.0999999999995</v>
-      </c>
-      <c r="K127" t="n">
-        <v>18.7</v>
-      </c>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
@@ -3936,7 +3326,11 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr"/>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Skoda Kodiaq I (4x4)</t>
+        </is>
+      </c>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
@@ -3944,7 +3338,6 @@
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
-      <c r="K128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
@@ -3961,15 +3354,8 @@
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
-      <c r="I129" t="n">
-        <v>6361.4</v>
-      </c>
-      <c r="J129" t="n">
-        <v>0</v>
-      </c>
-      <c r="K129" t="n">
-        <v>0</v>
-      </c>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
@@ -3986,15 +3372,8 @@
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr"/>
-      <c r="I130" t="n">
-        <v>6043.5</v>
-      </c>
-      <c r="J130" t="n">
-        <v>0</v>
-      </c>
-      <c r="K130" t="n">
-        <v>0</v>
-      </c>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n"/>
@@ -4011,15 +3390,8 @@
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
-      <c r="I131" t="n">
-        <v>5725.599999999999</v>
-      </c>
-      <c r="J131" t="n">
-        <v>0</v>
-      </c>
-      <c r="K131" t="n">
-        <v>0</v>
-      </c>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n"/>
@@ -4036,15 +3408,8 @@
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr"/>
-      <c r="I132" t="n">
-        <v>5089.8</v>
-      </c>
-      <c r="J132" t="n">
-        <v>0</v>
-      </c>
-      <c r="K132" t="n">
-        <v>0</v>
-      </c>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
@@ -4061,15 +3426,8 @@
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
-      <c r="I133" t="n">
-        <v>4453.15</v>
-      </c>
-      <c r="J133" t="n">
-        <v>0</v>
-      </c>
-      <c r="K133" t="n">
-        <v>0</v>
-      </c>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n"/>
@@ -4086,15 +3444,8 @@
       <c r="F134" t="inlineStr"/>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="inlineStr"/>
-      <c r="I134" t="n">
-        <v>4453.15</v>
-      </c>
-      <c r="J134" t="n">
-        <v>0</v>
-      </c>
-      <c r="K134" t="n">
-        <v>0</v>
-      </c>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
@@ -4107,15 +3458,38 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr"/>
-      <c r="D135" t="inlineStr"/>
-      <c r="E135" t="inlineStr"/>
-      <c r="F135" t="inlineStr"/>
-      <c r="G135" t="inlineStr"/>
-      <c r="H135" t="inlineStr"/>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Nissan X-Trail III rest.</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Nissan X-Trail</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Haval F7X / Nissan X-Trail</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Haval F7X  4WD</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Nissan X-Trail AT</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nissan Xtrail </t>
+        </is>
+      </c>
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr"/>
-      <c r="K135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n"/>
@@ -4142,15 +3516,8 @@
       <c r="H136" t="n">
         <v>3900</v>
       </c>
-      <c r="I136" t="n">
-        <v>3470</v>
-      </c>
-      <c r="J136" t="n">
-        <v>2891.4</v>
-      </c>
-      <c r="K136" t="n">
-        <v>45.45</v>
-      </c>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n"/>
@@ -4177,15 +3544,8 @@
       <c r="H137" t="n">
         <v>3900</v>
       </c>
-      <c r="I137" t="n">
-        <v>3470</v>
-      </c>
-      <c r="J137" t="n">
-        <v>2573.5</v>
-      </c>
-      <c r="K137" t="n">
-        <v>42.58</v>
-      </c>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n"/>
@@ -4212,15 +3572,8 @@
       <c r="H138" t="n">
         <v>3700</v>
       </c>
-      <c r="I138" t="n">
-        <v>3470</v>
-      </c>
-      <c r="J138" t="n">
-        <v>2255.599999999999</v>
-      </c>
-      <c r="K138" t="n">
-        <v>39.39</v>
-      </c>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n"/>
@@ -4247,15 +3600,8 @@
       <c r="H139" t="n">
         <v>3700</v>
       </c>
-      <c r="I139" t="n">
-        <v>3470</v>
-      </c>
-      <c r="J139" t="n">
-        <v>1619.8</v>
-      </c>
-      <c r="K139" t="n">
-        <v>31.82</v>
-      </c>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n"/>
@@ -4282,15 +3628,8 @@
       <c r="H140" t="n">
         <v>2700</v>
       </c>
-      <c r="I140" t="n">
-        <v>2700</v>
-      </c>
-      <c r="J140" t="n">
-        <v>1753.15</v>
-      </c>
-      <c r="K140" t="n">
-        <v>39.37</v>
-      </c>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n"/>
@@ -4317,15 +3656,8 @@
       <c r="H141" t="n">
         <v>2700</v>
       </c>
-      <c r="I141" t="n">
-        <v>2700</v>
-      </c>
-      <c r="J141" t="n">
-        <v>1753.15</v>
-      </c>
-      <c r="K141" t="n">
-        <v>39.37</v>
-      </c>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
@@ -4338,15 +3670,34 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C142" t="inlineStr"/>
-      <c r="D142" t="inlineStr"/>
-      <c r="E142" t="inlineStr"/>
-      <c r="F142" t="inlineStr"/>
-      <c r="G142" t="inlineStr"/>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Volkswagen Caravelle T6 Di; Hyundai H-1 II rest. 2</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Hyundai Staria</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Volkswagen Caravelle</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Hyundai H-1 AT</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>Hyundai Grand Starex AT</t>
+        </is>
+      </c>
       <c r="H142" t="inlineStr"/>
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
-      <c r="K142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n"/>
@@ -4371,15 +3722,8 @@
         <v>8670</v>
       </c>
       <c r="H143" t="inlineStr"/>
-      <c r="I143" t="n">
-        <v>5788.5</v>
-      </c>
-      <c r="J143" t="n">
-        <v>0</v>
-      </c>
-      <c r="K143" t="n">
-        <v>0</v>
-      </c>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n"/>
@@ -4404,15 +3748,8 @@
         <v>8170</v>
       </c>
       <c r="H144" t="inlineStr"/>
-      <c r="I144" t="n">
-        <v>5499.5</v>
-      </c>
-      <c r="J144" t="n">
-        <v>0</v>
-      </c>
-      <c r="K144" t="n">
-        <v>0</v>
-      </c>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n"/>
@@ -4437,15 +3774,8 @@
         <v>7470</v>
       </c>
       <c r="H145" t="inlineStr"/>
-      <c r="I145" t="n">
-        <v>5209.65</v>
-      </c>
-      <c r="J145" t="n">
-        <v>0</v>
-      </c>
-      <c r="K145" t="n">
-        <v>0</v>
-      </c>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n"/>
@@ -4470,15 +3800,8 @@
         <v>7470</v>
       </c>
       <c r="H146" t="inlineStr"/>
-      <c r="I146" t="n">
-        <v>4630.8</v>
-      </c>
-      <c r="J146" t="n">
-        <v>0</v>
-      </c>
-      <c r="K146" t="n">
-        <v>0</v>
-      </c>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n"/>
@@ -4503,15 +3826,8 @@
         <v>6970</v>
       </c>
       <c r="H147" t="inlineStr"/>
-      <c r="I147" t="n">
-        <v>4051.95</v>
-      </c>
-      <c r="J147" t="n">
-        <v>0</v>
-      </c>
-      <c r="K147" t="n">
-        <v>0</v>
-      </c>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n"/>
@@ -4536,15 +3852,8 @@
         <v>6970</v>
       </c>
       <c r="H148" t="inlineStr"/>
-      <c r="I148" t="n">
-        <v>4051.95</v>
-      </c>
-      <c r="J148" t="n">
-        <v>0</v>
-      </c>
-      <c r="K148" t="n">
-        <v>0</v>
-      </c>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
@@ -4565,7 +3874,6 @@
       <c r="H149" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr"/>
-      <c r="K149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n"/>
@@ -4582,15 +3890,8 @@
       <c r="F150" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr"/>
-      <c r="I150" t="n">
-        <v>7235.2</v>
-      </c>
-      <c r="J150" t="n">
-        <v>0</v>
-      </c>
-      <c r="K150" t="n">
-        <v>0</v>
-      </c>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n"/>
@@ -4607,15 +3908,8 @@
       <c r="F151" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr"/>
-      <c r="I151" t="n">
-        <v>6873.95</v>
-      </c>
-      <c r="J151" t="n">
-        <v>0</v>
-      </c>
-      <c r="K151" t="n">
-        <v>0</v>
-      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n"/>
@@ -4632,15 +3926,8 @@
       <c r="F152" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="inlineStr"/>
-      <c r="I152" t="n">
-        <v>6511.849999999999</v>
-      </c>
-      <c r="J152" t="n">
-        <v>0</v>
-      </c>
-      <c r="K152" t="n">
-        <v>0</v>
-      </c>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n"/>
@@ -4657,15 +3944,8 @@
       <c r="F153" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="inlineStr"/>
-      <c r="I153" t="n">
-        <v>5788.5</v>
-      </c>
-      <c r="J153" t="n">
-        <v>0</v>
-      </c>
-      <c r="K153" t="n">
-        <v>0</v>
-      </c>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n"/>
@@ -4682,15 +3962,8 @@
       <c r="F154" t="inlineStr"/>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr"/>
-      <c r="I154" t="n">
-        <v>5065.15</v>
-      </c>
-      <c r="J154" t="n">
-        <v>0</v>
-      </c>
-      <c r="K154" t="n">
-        <v>0</v>
-      </c>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n"/>
@@ -4707,15 +3980,8 @@
       <c r="F155" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr"/>
-      <c r="I155" t="n">
-        <v>5065.15</v>
-      </c>
-      <c r="J155" t="n">
-        <v>0</v>
-      </c>
-      <c r="K155" t="n">
-        <v>0</v>
-      </c>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="22">

</xml_diff>

<commit_message>
step 2 "with car names" done (next - car names for MIN column)
</commit_message>
<xml_diff>
--- a/outputs/analysiss.xlsx
+++ b/outputs/analysiss.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J155"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,27 +472,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RENT-MOTORS-22-02-24</t>
+          <t>RENT-MOTORS-01-03-24</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>REX-RENT-22-02-24</t>
+          <t>REX-RENT-01-03-24</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>A-ARENDA-22-02-24</t>
+          <t>A-ARENDA-01-03-24</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ALMAK-22-02-24</t>
+          <t>ALMAK-01-03-24</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>STORLET-22-02-24</t>
+          <t>STORLET-01-03-24</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -503,6 +503,11 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DELTA</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DELTA %</t>
         </is>
       </c>
     </row>
@@ -533,6 +538,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
@@ -542,7 +548,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2238.9</v>
+        <v>2634</v>
       </c>
       <c r="D3" t="n">
         <v>1750</v>
@@ -551,8 +557,15 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>1750</v>
+      </c>
+      <c r="J3" t="n">
+        <v>884</v>
+      </c>
+      <c r="K3" t="n">
+        <v>33.56112376613515</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
@@ -562,7 +575,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2127.55</v>
+        <v>2503</v>
       </c>
       <c r="D4" t="n">
         <v>1750</v>
@@ -571,8 +584,15 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>1750</v>
+      </c>
+      <c r="J4" t="n">
+        <v>753</v>
+      </c>
+      <c r="K4" t="n">
+        <v>30.08389932081502</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
@@ -582,7 +602,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2015.35</v>
+        <v>2371</v>
       </c>
       <c r="D5" t="n">
         <v>1500</v>
@@ -591,8 +611,15 @@
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J5" t="n">
+        <v>871</v>
+      </c>
+      <c r="K5" t="n">
+        <v>36.73555461830451</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -602,7 +629,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1858.95</v>
+        <v>2187</v>
       </c>
       <c r="D6" t="n">
         <v>1500</v>
@@ -611,8 +638,15 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J6" t="n">
+        <v>687</v>
+      </c>
+      <c r="K6" t="n">
+        <v>31.41289437585734</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
@@ -622,7 +656,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1746.75</v>
+        <v>2055</v>
       </c>
       <c r="D7" t="n">
         <v>1500</v>
@@ -631,8 +665,15 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J7" t="n">
+        <v>555</v>
+      </c>
+      <c r="K7" t="n">
+        <v>27.00729927007299</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
@@ -642,7 +683,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1679.6</v>
+        <v>1976</v>
       </c>
       <c r="D8" t="n">
         <v>1450</v>
@@ -651,8 +692,15 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>1450</v>
+      </c>
+      <c r="J8" t="n">
+        <v>526</v>
+      </c>
+      <c r="K8" t="n">
+        <v>26.61943319838057</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -673,6 +721,7 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
@@ -682,15 +731,22 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2798.2</v>
+        <v>3292</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>3292</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -700,15 +756,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2658.8</v>
+        <v>3128</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>3128</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -718,15 +781,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2518.55</v>
+        <v>2963</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>2963</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
@@ -736,15 +806,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2323.05</v>
+        <v>2733</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>2733</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
@@ -754,15 +831,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2182.8</v>
+        <v>2568</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>2568</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
@@ -772,15 +856,22 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2098.65</v>
+        <v>2469</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>2469</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -801,6 +892,7 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
@@ -817,8 +909,13 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
@@ -835,8 +932,13 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
@@ -853,8 +955,13 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
@@ -871,8 +978,13 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
@@ -889,8 +1001,13 @@
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
@@ -907,8 +1024,13 @@
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -937,6 +1059,7 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -946,7 +1069,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3280.15</v>
+        <v>3859</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -955,8 +1078,15 @@
         <v>3470</v>
       </c>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>3470</v>
+      </c>
+      <c r="J24" t="n">
+        <v>389</v>
+      </c>
+      <c r="K24" t="n">
+        <v>10.08033169214823</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
@@ -966,7 +1096,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3116.95</v>
+        <v>3667</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
@@ -975,8 +1105,15 @@
         <v>3270</v>
       </c>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>3270</v>
+      </c>
+      <c r="J25" t="n">
+        <v>397</v>
+      </c>
+      <c r="K25" t="n">
+        <v>10.82628851922552</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
@@ -986,7 +1123,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2952.9</v>
+        <v>3474</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -995,8 +1132,15 @@
         <v>2970</v>
       </c>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
+      <c r="I26" t="n">
+        <v>2970</v>
+      </c>
+      <c r="J26" t="n">
+        <v>504</v>
+      </c>
+      <c r="K26" t="n">
+        <v>14.50777202072539</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
@@ -1006,7 +1150,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2624.8</v>
+        <v>3088</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
@@ -1015,8 +1159,15 @@
         <v>2970</v>
       </c>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="I27" t="n">
+        <v>2970</v>
+      </c>
+      <c r="J27" t="n">
+        <v>118</v>
+      </c>
+      <c r="K27" t="n">
+        <v>3.821243523316062</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
@@ -1026,7 +1177,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2296.7</v>
+        <v>2702</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -1035,8 +1186,15 @@
         <v>2870</v>
       </c>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
+      <c r="I28" t="n">
+        <v>2702</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
@@ -1046,7 +1204,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2296.7</v>
+        <v>2702</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
@@ -1055,8 +1213,15 @@
         <v>2870</v>
       </c>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
+      <c r="I29" t="n">
+        <v>2702</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -1081,6 +1246,7 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
@@ -1090,15 +1256,22 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2431.85</v>
+        <v>2861</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="I31" t="n">
+        <v>2861</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
@@ -1108,15 +1281,22 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2310.3</v>
+        <v>2718</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
+      <c r="I32" t="n">
+        <v>2718</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
@@ -1126,15 +1306,22 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2188.75</v>
+        <v>2575</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
+      <c r="I33" t="n">
+        <v>2575</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
@@ -1144,15 +1331,22 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2018.75</v>
+        <v>2375</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
+      <c r="I34" t="n">
+        <v>2375</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
@@ -1162,15 +1356,22 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1897.2</v>
+        <v>2232</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
+      <c r="I35" t="n">
+        <v>2232</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
@@ -1180,15 +1381,22 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1824.1</v>
+        <v>2146</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>2146</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -1216,7 +1424,11 @@
           <t>Сhangan Alsvin / Renault Logan</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Hyundai  Solaris 1.6  AT</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr">
         <is>
           <t>Hyundai Solaris II Promo</t>
@@ -1229,6 +1441,7 @@
       </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
@@ -1238,7 +1451,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3039.6</v>
+        <v>3576</v>
       </c>
       <c r="D38" t="n">
         <v>2200</v>
@@ -1246,15 +1459,24 @@
       <c r="E38" t="n">
         <v>3200</v>
       </c>
-      <c r="F38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>3150</v>
+      </c>
       <c r="G38" t="n">
         <v>2570</v>
       </c>
       <c r="H38" t="n">
         <v>2000</v>
       </c>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1576</v>
+      </c>
+      <c r="K38" t="n">
+        <v>44.07158836689038</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
@@ -1264,7 +1486,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2888.3</v>
+        <v>3398</v>
       </c>
       <c r="D39" t="n">
         <v>2200</v>
@@ -1272,15 +1494,24 @@
       <c r="E39" t="n">
         <v>2816.67</v>
       </c>
-      <c r="F39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>2830</v>
+      </c>
       <c r="G39" t="n">
         <v>2470</v>
       </c>
       <c r="H39" t="n">
         <v>2000</v>
       </c>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1398</v>
+      </c>
+      <c r="K39" t="n">
+        <v>41.14184814596822</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
@@ -1290,7 +1521,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2736.15</v>
+        <v>3219</v>
       </c>
       <c r="D40" t="n">
         <v>1900</v>
@@ -1298,15 +1529,24 @@
       <c r="E40" t="n">
         <v>2321.43</v>
       </c>
-      <c r="F40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>2710</v>
+      </c>
       <c r="G40" t="n">
         <v>2270</v>
       </c>
       <c r="H40" t="n">
         <v>1800</v>
       </c>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+      <c r="I40" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1419</v>
+      </c>
+      <c r="K40" t="n">
+        <v>44.08201304753029</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
@@ -1316,7 +1556,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2523.65</v>
+        <v>2969</v>
       </c>
       <c r="D41" t="n">
         <v>1900</v>
@@ -1324,15 +1564,24 @@
       <c r="E41" t="n">
         <v>2285.71</v>
       </c>
-      <c r="F41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>2710</v>
+      </c>
       <c r="G41" t="n">
         <v>2270</v>
       </c>
       <c r="H41" t="n">
         <v>1800</v>
       </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+      <c r="I41" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1169</v>
+      </c>
+      <c r="K41" t="n">
+        <v>39.37352643987875</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
@@ -1342,7 +1591,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2371.5</v>
+        <v>2790</v>
       </c>
       <c r="D42" t="n">
         <v>1900</v>
@@ -1350,15 +1599,24 @@
       <c r="E42" t="n">
         <v>2273.81</v>
       </c>
-      <c r="F42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>2520</v>
+      </c>
       <c r="G42" t="n">
         <v>2170</v>
       </c>
       <c r="H42" t="n">
         <v>1500</v>
       </c>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J42" t="n">
+        <v>1290</v>
+      </c>
+      <c r="K42" t="n">
+        <v>46.23655913978494</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
@@ -1368,7 +1626,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2279.7</v>
+        <v>2682</v>
       </c>
       <c r="D43" t="n">
         <v>1800</v>
@@ -1376,15 +1634,24 @@
       <c r="E43" t="n">
         <v>2216.67</v>
       </c>
-      <c r="F43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>2438</v>
+      </c>
       <c r="G43" t="n">
         <v>2170</v>
       </c>
       <c r="H43" t="n">
         <v>1500</v>
       </c>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J43" t="n">
+        <v>1182</v>
+      </c>
+      <c r="K43" t="n">
+        <v>44.07158836689038</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1409,6 +1676,7 @@
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
@@ -1418,15 +1686,22 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2809.25</v>
+        <v>3305</v>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
+      <c r="I45" t="n">
+        <v>3305</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
@@ -1436,15 +1711,22 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2669</v>
+        <v>3140</v>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
+      <c r="I46" t="n">
+        <v>3140</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
@@ -1454,15 +1736,22 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2528.75</v>
+        <v>2975</v>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
+      <c r="I47" t="n">
+        <v>2975</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
@@ -1472,15 +1761,22 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2247.4</v>
+        <v>2644</v>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>2644</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
@@ -1490,15 +1786,22 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1966.9</v>
+        <v>2314</v>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>2314</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
@@ -1508,15 +1811,22 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1966.9</v>
+        <v>2314</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
+      <c r="I50" t="n">
+        <v>2314</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1534,7 +1844,11 @@
           <t>Volkswagen Polo VI; Skoda Rapid II</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Renault Logan.1</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
@@ -1549,6 +1863,7 @@
       </c>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
@@ -1558,9 +1873,11 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3511.35</v>
-      </c>
-      <c r="D52" t="inlineStr"/>
+        <v>4131</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1950</v>
+      </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
@@ -1569,8 +1886,15 @@
       <c r="H52" t="n">
         <v>1800</v>
       </c>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
+      <c r="I52" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2331</v>
+      </c>
+      <c r="K52" t="n">
+        <v>56.42701525054466</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
@@ -1580,9 +1904,11 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3336.25</v>
-      </c>
-      <c r="D53" t="inlineStr"/>
+        <v>3925</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1950</v>
+      </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
@@ -1591,8 +1917,15 @@
       <c r="H53" t="n">
         <v>1800</v>
       </c>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
+      <c r="I53" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2125</v>
+      </c>
+      <c r="K53" t="n">
+        <v>54.14012738853503</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
@@ -1602,9 +1935,11 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3160.3</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+        <v>3718</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1700</v>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
@@ -1613,8 +1948,15 @@
       <c r="H54" t="n">
         <v>1600</v>
       </c>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
+      <c r="I54" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J54" t="n">
+        <v>2118</v>
+      </c>
+      <c r="K54" t="n">
+        <v>56.96611081226466</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
@@ -1624,9 +1966,11 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2809.25</v>
-      </c>
-      <c r="D55" t="inlineStr"/>
+        <v>3305</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1700</v>
+      </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
@@ -1635,8 +1979,15 @@
       <c r="H55" t="n">
         <v>1600</v>
       </c>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
+      <c r="I55" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1705</v>
+      </c>
+      <c r="K55" t="n">
+        <v>51.58850226928896</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n"/>
@@ -1646,9 +1997,11 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2458.2</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+        <v>2892</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1700</v>
+      </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
@@ -1657,8 +2010,15 @@
       <c r="H56" t="n">
         <v>1400</v>
       </c>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
+      <c r="I56" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1492</v>
+      </c>
+      <c r="K56" t="n">
+        <v>51.59059474412172</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
@@ -1668,9 +2028,11 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2458.2</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+        <v>2892</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1600</v>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
@@ -1679,8 +2041,15 @@
       <c r="H57" t="n">
         <v>1400</v>
       </c>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
+      <c r="I57" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1492</v>
+      </c>
+      <c r="K57" t="n">
+        <v>51.59059474412172</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1713,6 +2082,7 @@
       </c>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
@@ -1722,7 +2092,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3136.5</v>
+        <v>3690</v>
       </c>
       <c r="D59" t="n">
         <v>3000</v>
@@ -1733,8 +2103,15 @@
       <c r="H59" t="n">
         <v>1800</v>
       </c>
-      <c r="I59" t="inlineStr"/>
-      <c r="J59" t="inlineStr"/>
+      <c r="I59" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1890</v>
+      </c>
+      <c r="K59" t="n">
+        <v>51.21951219512195</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
@@ -1744,7 +2121,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2980.1</v>
+        <v>3506</v>
       </c>
       <c r="D60" t="n">
         <v>3000</v>
@@ -1755,8 +2132,15 @@
       <c r="H60" t="n">
         <v>1800</v>
       </c>
-      <c r="I60" t="inlineStr"/>
-      <c r="J60" t="inlineStr"/>
+      <c r="I60" t="n">
+        <v>1800</v>
+      </c>
+      <c r="J60" t="n">
+        <v>1706</v>
+      </c>
+      <c r="K60" t="n">
+        <v>48.6594409583571</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
@@ -1766,7 +2150,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2822.85</v>
+        <v>3321</v>
       </c>
       <c r="D61" t="n">
         <v>2600</v>
@@ -1777,8 +2161,15 @@
       <c r="H61" t="n">
         <v>1600</v>
       </c>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
+      <c r="I61" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J61" t="n">
+        <v>1721</v>
+      </c>
+      <c r="K61" t="n">
+        <v>51.82174043962662</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
@@ -1788,7 +2179,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2509.2</v>
+        <v>2952</v>
       </c>
       <c r="D62" t="n">
         <v>2600</v>
@@ -1799,8 +2190,15 @@
       <c r="H62" t="n">
         <v>1600</v>
       </c>
-      <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
+      <c r="I62" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1352</v>
+      </c>
+      <c r="K62" t="n">
+        <v>45.79945799457995</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
@@ -1810,7 +2208,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2195.55</v>
+        <v>2583</v>
       </c>
       <c r="D63" t="n">
         <v>2600</v>
@@ -1821,8 +2219,15 @@
       <c r="H63" t="n">
         <v>1200</v>
       </c>
-      <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
+      <c r="I63" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J63" t="n">
+        <v>1383</v>
+      </c>
+      <c r="K63" t="n">
+        <v>53.54239256678282</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n"/>
@@ -1832,7 +2237,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2195.55</v>
+        <v>2583</v>
       </c>
       <c r="D64" t="n">
         <v>2100</v>
@@ -1843,8 +2248,15 @@
       <c r="H64" t="n">
         <v>1200</v>
       </c>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="inlineStr"/>
+      <c r="I64" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J64" t="n">
+        <v>1383</v>
+      </c>
+      <c r="K64" t="n">
+        <v>53.54239256678282</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -1877,6 +2289,7 @@
       </c>
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
@@ -1886,7 +2299,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>3689.85</v>
+        <v>4341</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
@@ -1897,8 +2310,15 @@
       <c r="H66" t="n">
         <v>2100</v>
       </c>
-      <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr"/>
+      <c r="I66" t="n">
+        <v>2100</v>
+      </c>
+      <c r="J66" t="n">
+        <v>2241</v>
+      </c>
+      <c r="K66" t="n">
+        <v>51.62404975812025</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
@@ -1908,7 +2328,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>3505.4</v>
+        <v>4124</v>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
@@ -1919,8 +2339,15 @@
       <c r="H67" t="n">
         <v>2100</v>
       </c>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
+      <c r="I67" t="n">
+        <v>2100</v>
+      </c>
+      <c r="J67" t="n">
+        <v>2024</v>
+      </c>
+      <c r="K67" t="n">
+        <v>49.07856450048497</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
@@ -1930,7 +2357,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>3320.95</v>
+        <v>3907</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
@@ -1941,8 +2368,15 @@
       <c r="H68" t="n">
         <v>1900</v>
       </c>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
+      <c r="I68" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J68" t="n">
+        <v>2007</v>
+      </c>
+      <c r="K68" t="n">
+        <v>51.36933708727924</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
@@ -1952,7 +2386,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2952.05</v>
+        <v>3473</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
@@ -1963,8 +2397,15 @@
       <c r="H69" t="n">
         <v>1900</v>
       </c>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
+      <c r="I69" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J69" t="n">
+        <v>1573</v>
+      </c>
+      <c r="K69" t="n">
+        <v>45.29225453498416</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
@@ -1974,7 +2415,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2583.15</v>
+        <v>3039</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
@@ -1985,8 +2426,15 @@
       <c r="H70" t="n">
         <v>1500</v>
       </c>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
+      <c r="I70" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J70" t="n">
+        <v>1539</v>
+      </c>
+      <c r="K70" t="n">
+        <v>50.6416584402764</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
@@ -1996,7 +2444,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2583.15</v>
+        <v>3039</v>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
@@ -2007,8 +2455,15 @@
       <c r="H71" t="n">
         <v>1500</v>
       </c>
-      <c r="I71" t="inlineStr"/>
-      <c r="J71" t="inlineStr"/>
+      <c r="I71" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1539</v>
+      </c>
+      <c r="K71" t="n">
+        <v>50.6416584402764</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -2031,7 +2486,11 @@
           <t>Hyundai Sonata</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>KIA K5 / Hyundai Sonata</t>
+        </is>
+      </c>
       <c r="F72" t="inlineStr">
         <is>
           <t>Hyundai Sonata VIII 2.5</t>
@@ -2049,6 +2508,7 @@
       </c>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
@@ -2058,12 +2518,14 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>4250.849999999999</v>
+        <v>5001</v>
       </c>
       <c r="D73" t="n">
         <v>3800</v>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>6308</v>
+      </c>
       <c r="F73" t="n">
         <v>3510</v>
       </c>
@@ -2073,8 +2535,15 @@
       <c r="H73" t="n">
         <v>2500</v>
       </c>
-      <c r="I73" t="inlineStr"/>
-      <c r="J73" t="inlineStr"/>
+      <c r="I73" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J73" t="n">
+        <v>2501</v>
+      </c>
+      <c r="K73" t="n">
+        <v>50.00999800039992</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
@@ -2084,12 +2553,14 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>4038.35</v>
+        <v>4751</v>
       </c>
       <c r="D74" t="n">
         <v>3800</v>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>5974.33</v>
+      </c>
       <c r="F74" t="n">
         <v>3510</v>
       </c>
@@ -2099,8 +2570,15 @@
       <c r="H74" t="n">
         <v>2500</v>
       </c>
-      <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
+      <c r="I74" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J74" t="n">
+        <v>2251</v>
+      </c>
+      <c r="K74" t="n">
+        <v>47.37949905283098</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
@@ -2110,12 +2588,14 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3825.85</v>
+        <v>4501</v>
       </c>
       <c r="D75" t="n">
         <v>3200</v>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>5304</v>
+      </c>
       <c r="F75" t="n">
         <v>3510</v>
       </c>
@@ -2125,8 +2605,15 @@
       <c r="H75" t="n">
         <v>2400</v>
       </c>
-      <c r="I75" t="inlineStr"/>
-      <c r="J75" t="inlineStr"/>
+      <c r="I75" t="n">
+        <v>2400</v>
+      </c>
+      <c r="J75" t="n">
+        <v>2101</v>
+      </c>
+      <c r="K75" t="n">
+        <v>46.67851588535881</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
@@ -2136,12 +2623,14 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>3400.85</v>
+        <v>4001</v>
       </c>
       <c r="D76" t="n">
         <v>3200</v>
       </c>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>5268.21</v>
+      </c>
       <c r="F76" t="n">
         <v>3510</v>
       </c>
@@ -2151,8 +2640,15 @@
       <c r="H76" t="n">
         <v>2400</v>
       </c>
-      <c r="I76" t="inlineStr"/>
-      <c r="J76" t="inlineStr"/>
+      <c r="I76" t="n">
+        <v>2400</v>
+      </c>
+      <c r="J76" t="n">
+        <v>1601</v>
+      </c>
+      <c r="K76" t="n">
+        <v>40.01499625093727</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
@@ -2162,12 +2658,14 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2975.85</v>
+        <v>3501</v>
       </c>
       <c r="D77" t="n">
         <v>3200</v>
       </c>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>5256.33</v>
+      </c>
       <c r="F77" t="n">
         <v>3320</v>
       </c>
@@ -2177,8 +2675,15 @@
       <c r="H77" t="n">
         <v>1900</v>
       </c>
-      <c r="I77" t="inlineStr"/>
-      <c r="J77" t="inlineStr"/>
+      <c r="I77" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J77" t="n">
+        <v>1601</v>
+      </c>
+      <c r="K77" t="n">
+        <v>45.72979148814624</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
@@ -2188,14 +2693,16 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2975.85</v>
+        <v>3501</v>
       </c>
       <c r="D78" t="n">
         <v>2800</v>
       </c>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>4674.17</v>
+      </c>
       <c r="F78" t="n">
-        <v>3320</v>
+        <v>3634</v>
       </c>
       <c r="G78" t="n">
         <v>3170</v>
@@ -2203,8 +2710,15 @@
       <c r="H78" t="n">
         <v>1900</v>
       </c>
-      <c r="I78" t="inlineStr"/>
-      <c r="J78" t="inlineStr"/>
+      <c r="I78" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J78" t="n">
+        <v>1601</v>
+      </c>
+      <c r="K78" t="n">
+        <v>45.72979148814624</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -2225,6 +2739,7 @@
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
@@ -2234,15 +2749,22 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>4722.599999999999</v>
+        <v>5556</v>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="inlineStr"/>
-      <c r="J80" t="inlineStr"/>
+      <c r="I80" t="n">
+        <v>5556</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
@@ -2252,15 +2774,22 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4487.15</v>
+        <v>5279</v>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
-      <c r="I81" t="inlineStr"/>
-      <c r="J81" t="inlineStr"/>
+      <c r="I81" t="n">
+        <v>5279</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
@@ -2270,15 +2799,22 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>4250.849999999999</v>
+        <v>5001</v>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
-      <c r="I82" t="inlineStr"/>
-      <c r="J82" t="inlineStr"/>
+      <c r="I82" t="n">
+        <v>5001</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
@@ -2288,15 +2824,22 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3778.25</v>
+        <v>4445</v>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr"/>
+      <c r="I83" t="n">
+        <v>4445</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
@@ -2306,15 +2849,22 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3306.5</v>
+        <v>3890</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr"/>
+      <c r="I84" t="n">
+        <v>3890</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
@@ -2324,15 +2874,22 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3306.5</v>
+        <v>3890</v>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr"/>
+      <c r="I85" t="n">
+        <v>3890</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -2369,6 +2926,7 @@
       </c>
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
@@ -2378,7 +2936,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>3433.15</v>
+        <v>4039</v>
       </c>
       <c r="D87" t="n">
         <v>3300</v>
@@ -2391,8 +2949,15 @@
       <c r="H87" t="n">
         <v>2200</v>
       </c>
-      <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
+      <c r="I87" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1839</v>
+      </c>
+      <c r="K87" t="n">
+        <v>45.53107204753652</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
@@ -2402,7 +2967,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3262.3</v>
+        <v>3838</v>
       </c>
       <c r="D88" t="n">
         <v>3300</v>
@@ -2415,8 +2980,15 @@
       <c r="H88" t="n">
         <v>2200</v>
       </c>
-      <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
+      <c r="I88" t="n">
+        <v>2200</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1638</v>
+      </c>
+      <c r="K88" t="n">
+        <v>42.67847837415321</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
@@ -2426,7 +2998,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3090.6</v>
+        <v>3636</v>
       </c>
       <c r="D89" t="n">
         <v>2900</v>
@@ -2439,8 +3011,15 @@
       <c r="H89" t="n">
         <v>1900</v>
       </c>
-      <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr"/>
+      <c r="I89" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J89" t="n">
+        <v>1736</v>
+      </c>
+      <c r="K89" t="n">
+        <v>47.74477447744774</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
@@ -2450,7 +3029,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2747.2</v>
+        <v>3232</v>
       </c>
       <c r="D90" t="n">
         <v>2900</v>
@@ -2463,8 +3042,15 @@
       <c r="H90" t="n">
         <v>1900</v>
       </c>
-      <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
+      <c r="I90" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J90" t="n">
+        <v>1332</v>
+      </c>
+      <c r="K90" t="n">
+        <v>41.21287128712871</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
@@ -2474,7 +3060,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2575.5</v>
+        <v>3030</v>
       </c>
       <c r="D91" t="n">
         <v>2900</v>
@@ -2487,8 +3073,15 @@
       <c r="H91" t="n">
         <v>1600</v>
       </c>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
+      <c r="I91" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J91" t="n">
+        <v>1430</v>
+      </c>
+      <c r="K91" t="n">
+        <v>47.1947194719472</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
@@ -2498,7 +3091,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2403.8</v>
+        <v>2828</v>
       </c>
       <c r="D92" t="n">
         <v>2200</v>
@@ -2511,8 +3104,15 @@
       <c r="H92" t="n">
         <v>1600</v>
       </c>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
+      <c r="I92" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J92" t="n">
+        <v>1228</v>
+      </c>
+      <c r="K92" t="n">
+        <v>43.42291371994342</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -2545,6 +3145,7 @@
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
@@ -2554,7 +3155,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3813.95</v>
+        <v>4487</v>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="n">
@@ -2565,8 +3166,15 @@
         <v>3670</v>
       </c>
       <c r="H94" t="inlineStr"/>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
+      <c r="I94" t="n">
+        <v>3670</v>
+      </c>
+      <c r="J94" t="n">
+        <v>817</v>
+      </c>
+      <c r="K94" t="n">
+        <v>18.20815689770448</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
@@ -2576,7 +3184,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>3623.55</v>
+        <v>4263</v>
       </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="n">
@@ -2587,8 +3195,15 @@
         <v>3470</v>
       </c>
       <c r="H95" t="inlineStr"/>
-      <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr"/>
+      <c r="I95" t="n">
+        <v>3470</v>
+      </c>
+      <c r="J95" t="n">
+        <v>793</v>
+      </c>
+      <c r="K95" t="n">
+        <v>18.6019235280319</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
@@ -2598,7 +3213,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>3433.15</v>
+        <v>4039</v>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="n">
@@ -2609,8 +3224,15 @@
         <v>3170</v>
       </c>
       <c r="H96" t="inlineStr"/>
-      <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr"/>
+      <c r="I96" t="n">
+        <v>2871.43</v>
+      </c>
+      <c r="J96" t="n">
+        <v>1167.57</v>
+      </c>
+      <c r="K96" t="n">
+        <v>28.90740282248082</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
@@ -2620,7 +3242,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>3051.5</v>
+        <v>3590</v>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
@@ -2631,8 +3253,15 @@
         <v>3170</v>
       </c>
       <c r="H97" t="inlineStr"/>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
+      <c r="I97" t="n">
+        <v>2835.71</v>
+      </c>
+      <c r="J97" t="n">
+        <v>754.29</v>
+      </c>
+      <c r="K97" t="n">
+        <v>21.0108635097493</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
@@ -2642,7 +3271,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>2861.1</v>
+        <v>3366</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="n">
@@ -2653,8 +3282,15 @@
         <v>2970</v>
       </c>
       <c r="H98" t="inlineStr"/>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
+      <c r="I98" t="n">
+        <v>2823.81</v>
+      </c>
+      <c r="J98" t="n">
+        <v>542.1900000000001</v>
+      </c>
+      <c r="K98" t="n">
+        <v>16.1078431372549</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
@@ -2664,7 +3300,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2669.85</v>
+        <v>3141</v>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
@@ -2675,8 +3311,15 @@
         <v>2970</v>
       </c>
       <c r="H99" t="inlineStr"/>
-      <c r="I99" t="inlineStr"/>
-      <c r="J99" t="inlineStr"/>
+      <c r="I99" t="n">
+        <v>2816.67</v>
+      </c>
+      <c r="J99" t="n">
+        <v>324.3299999999999</v>
+      </c>
+      <c r="K99" t="n">
+        <v>10.32569245463228</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
@@ -2697,6 +3340,7 @@
       <c r="H100" t="inlineStr"/>
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
@@ -2713,8 +3357,13 @@
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
@@ -2731,8 +3380,13 @@
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
-      <c r="I102" t="inlineStr"/>
-      <c r="J102" t="inlineStr"/>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n"/>
@@ -2749,8 +3403,13 @@
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
-      <c r="I103" t="inlineStr"/>
-      <c r="J103" t="inlineStr"/>
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
@@ -2767,8 +3426,13 @@
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
-      <c r="I104" t="inlineStr"/>
-      <c r="J104" t="inlineStr"/>
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
@@ -2785,8 +3449,13 @@
       <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
-      <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr"/>
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n"/>
@@ -2803,8 +3472,13 @@
       <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr"/>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
@@ -2846,6 +3520,7 @@
       </c>
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n"/>
@@ -2855,7 +3530,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>3995.85</v>
+        <v>4701</v>
       </c>
       <c r="D108" t="n">
         <v>3700</v>
@@ -2870,8 +3545,15 @@
       <c r="H108" t="n">
         <v>3900</v>
       </c>
-      <c r="I108" t="inlineStr"/>
-      <c r="J108" t="inlineStr"/>
+      <c r="I108" t="n">
+        <v>3270</v>
+      </c>
+      <c r="J108" t="n">
+        <v>1431</v>
+      </c>
+      <c r="K108" t="n">
+        <v>30.44033184428845</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n"/>
@@ -2881,7 +3563,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3796.1</v>
+        <v>4466</v>
       </c>
       <c r="D109" t="n">
         <v>3700</v>
@@ -2896,8 +3578,15 @@
       <c r="H109" t="n">
         <v>3900</v>
       </c>
-      <c r="I109" t="inlineStr"/>
-      <c r="J109" t="inlineStr"/>
+      <c r="I109" t="n">
+        <v>3070</v>
+      </c>
+      <c r="J109" t="n">
+        <v>1396</v>
+      </c>
+      <c r="K109" t="n">
+        <v>31.25839677563815</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n"/>
@@ -2907,7 +3596,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>3596.35</v>
+        <v>4231</v>
       </c>
       <c r="D110" t="n">
         <v>3200</v>
@@ -2922,8 +3611,15 @@
       <c r="H110" t="n">
         <v>3500</v>
       </c>
-      <c r="I110" t="inlineStr"/>
-      <c r="J110" t="inlineStr"/>
+      <c r="I110" t="n">
+        <v>2870</v>
+      </c>
+      <c r="J110" t="n">
+        <v>1361</v>
+      </c>
+      <c r="K110" t="n">
+        <v>32.16733632710943</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n"/>
@@ -2933,7 +3629,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>3196.85</v>
+        <v>3761</v>
       </c>
       <c r="D111" t="n">
         <v>3200</v>
@@ -2948,8 +3644,15 @@
       <c r="H111" t="n">
         <v>3500</v>
       </c>
-      <c r="I111" t="inlineStr"/>
-      <c r="J111" t="inlineStr"/>
+      <c r="I111" t="n">
+        <v>2870</v>
+      </c>
+      <c r="J111" t="n">
+        <v>891</v>
+      </c>
+      <c r="K111" t="n">
+        <v>23.6905078436586</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n"/>
@@ -2959,7 +3662,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>2797.35</v>
+        <v>3291</v>
       </c>
       <c r="D112" t="n">
         <v>3200</v>
@@ -2974,8 +3677,15 @@
       <c r="H112" t="n">
         <v>2500</v>
       </c>
-      <c r="I112" t="inlineStr"/>
-      <c r="J112" t="inlineStr"/>
+      <c r="I112" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J112" t="n">
+        <v>791</v>
+      </c>
+      <c r="K112" t="n">
+        <v>24.03524764509268</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n"/>
@@ -2985,14 +3695,14 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>2797.35</v>
+        <v>3291</v>
       </c>
       <c r="D113" t="n">
         <v>2500</v>
       </c>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="n">
-        <v>3040</v>
+        <v>3192</v>
       </c>
       <c r="G113" t="n">
         <v>2670</v>
@@ -3000,8 +3710,15 @@
       <c r="H113" t="n">
         <v>2500</v>
       </c>
-      <c r="I113" t="inlineStr"/>
-      <c r="J113" t="inlineStr"/>
+      <c r="I113" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J113" t="n">
+        <v>791</v>
+      </c>
+      <c r="K113" t="n">
+        <v>24.03524764509268</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
@@ -3022,6 +3739,7 @@
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n"/>
@@ -3030,14 +3748,23 @@
           <t>r1</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr"/>
+      <c r="C115" t="n">
+        <v>6275</v>
+      </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
-      <c r="I115" t="inlineStr"/>
-      <c r="J115" t="inlineStr"/>
+      <c r="I115" t="n">
+        <v>6275</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n"/>
@@ -3046,14 +3773,23 @@
           <t>r3</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
+      <c r="C116" t="n">
+        <v>5962</v>
+      </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="inlineStr"/>
-      <c r="J116" t="inlineStr"/>
+      <c r="I116" t="n">
+        <v>5962</v>
+      </c>
+      <c r="J116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n"/>
@@ -3062,14 +3798,23 @@
           <t>r7</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>5648</v>
+      </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
-      <c r="I117" t="inlineStr"/>
-      <c r="J117" t="inlineStr"/>
+      <c r="I117" t="n">
+        <v>5648</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n"/>
@@ -3078,14 +3823,23 @@
           <t>r14</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr"/>
+      <c r="C118" t="n">
+        <v>5020</v>
+      </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
-      <c r="I118" t="inlineStr"/>
-      <c r="J118" t="inlineStr"/>
+      <c r="I118" t="n">
+        <v>5020</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n"/>
@@ -3094,14 +3848,23 @@
           <t>r21</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr"/>
+      <c r="C119" t="n">
+        <v>4393</v>
+      </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
-      <c r="I119" t="inlineStr"/>
-      <c r="J119" t="inlineStr"/>
+      <c r="I119" t="n">
+        <v>4393</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n"/>
@@ -3110,14 +3873,23 @@
           <t>r30</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" t="n">
+        <v>4393</v>
+      </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
-      <c r="I120" t="inlineStr"/>
-      <c r="J120" t="inlineStr"/>
+      <c r="I120" t="n">
+        <v>4393</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
@@ -3130,7 +3902,11 @@
           <t>car_name</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Haval JOLION I, Skoda Karoq I</t>
+        </is>
+      </c>
       <c r="D121" t="inlineStr">
         <is>
           <t>Haval Jolion</t>
@@ -3158,6 +3934,7 @@
       </c>
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n"/>
@@ -3166,7 +3943,9 @@
           <t>r1</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr"/>
+      <c r="C122" t="n">
+        <v>6275</v>
+      </c>
       <c r="D122" t="n">
         <v>3700</v>
       </c>
@@ -3182,8 +3961,15 @@
       <c r="H122" t="n">
         <v>3500</v>
       </c>
-      <c r="I122" t="inlineStr"/>
-      <c r="J122" t="inlineStr"/>
+      <c r="I122" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J122" t="n">
+        <v>3775</v>
+      </c>
+      <c r="K122" t="n">
+        <v>60.1593625498008</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n"/>
@@ -3192,7 +3978,9 @@
           <t>r3</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr"/>
+      <c r="C123" t="n">
+        <v>5962</v>
+      </c>
       <c r="D123" t="n">
         <v>3700</v>
       </c>
@@ -3208,8 +3996,15 @@
       <c r="H123" t="n">
         <v>3500</v>
       </c>
-      <c r="I123" t="inlineStr"/>
-      <c r="J123" t="inlineStr"/>
+      <c r="I123" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J123" t="n">
+        <v>3462</v>
+      </c>
+      <c r="K123" t="n">
+        <v>58.06776249580678</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n"/>
@@ -3218,7 +4013,9 @@
           <t>r7</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr"/>
+      <c r="C124" t="n">
+        <v>5648</v>
+      </c>
       <c r="D124" t="n">
         <v>3300</v>
       </c>
@@ -3234,8 +4031,15 @@
       <c r="H124" t="n">
         <v>3300</v>
       </c>
-      <c r="I124" t="inlineStr"/>
-      <c r="J124" t="inlineStr"/>
+      <c r="I124" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J124" t="n">
+        <v>3148</v>
+      </c>
+      <c r="K124" t="n">
+        <v>55.73654390934845</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n"/>
@@ -3244,7 +4048,9 @@
           <t>r14</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr"/>
+      <c r="C125" t="n">
+        <v>5020</v>
+      </c>
       <c r="D125" t="n">
         <v>3300</v>
       </c>
@@ -3260,8 +4066,15 @@
       <c r="H125" t="n">
         <v>3300</v>
       </c>
-      <c r="I125" t="inlineStr"/>
-      <c r="J125" t="inlineStr"/>
+      <c r="I125" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J125" t="n">
+        <v>2520</v>
+      </c>
+      <c r="K125" t="n">
+        <v>50.19920318725099</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n"/>
@@ -3270,7 +4083,9 @@
           <t>r21</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr"/>
+      <c r="C126" t="n">
+        <v>4393</v>
+      </c>
       <c r="D126" t="n">
         <v>3300</v>
       </c>
@@ -3286,8 +4101,15 @@
       <c r="H126" t="n">
         <v>2500</v>
       </c>
-      <c r="I126" t="inlineStr"/>
-      <c r="J126" t="inlineStr"/>
+      <c r="I126" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J126" t="n">
+        <v>1893</v>
+      </c>
+      <c r="K126" t="n">
+        <v>43.09128158433872</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n"/>
@@ -3296,7 +4118,9 @@
           <t>r30</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr"/>
+      <c r="C127" t="n">
+        <v>4393</v>
+      </c>
       <c r="D127" t="n">
         <v>2800</v>
       </c>
@@ -3304,7 +4128,7 @@
         <v>2816.67</v>
       </c>
       <c r="F127" t="n">
-        <v>2500</v>
+        <v>2718</v>
       </c>
       <c r="G127" t="n">
         <v>3270</v>
@@ -3312,8 +4136,15 @@
       <c r="H127" t="n">
         <v>2500</v>
       </c>
-      <c r="I127" t="inlineStr"/>
-      <c r="J127" t="inlineStr"/>
+      <c r="I127" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J127" t="n">
+        <v>1893</v>
+      </c>
+      <c r="K127" t="n">
+        <v>43.09128158433872</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
@@ -3338,6 +4169,7 @@
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n"/>
@@ -3347,15 +4179,22 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>6361.4</v>
+        <v>7484</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
-      <c r="I129" t="inlineStr"/>
-      <c r="J129" t="inlineStr"/>
+      <c r="I129" t="n">
+        <v>7484</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n"/>
@@ -3365,15 +4204,22 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>6043.5</v>
+        <v>7110</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr"/>
-      <c r="I130" t="inlineStr"/>
-      <c r="J130" t="inlineStr"/>
+      <c r="I130" t="n">
+        <v>7110</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n"/>
@@ -3383,15 +4229,22 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>5725.599999999999</v>
+        <v>6736</v>
       </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
-      <c r="I131" t="inlineStr"/>
-      <c r="J131" t="inlineStr"/>
+      <c r="I131" t="n">
+        <v>6736</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n"/>
@@ -3401,15 +4254,22 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>5089.8</v>
+        <v>5988</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr"/>
-      <c r="I132" t="inlineStr"/>
-      <c r="J132" t="inlineStr"/>
+      <c r="I132" t="n">
+        <v>5988</v>
+      </c>
+      <c r="J132" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n"/>
@@ -3419,15 +4279,22 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>4453.15</v>
+        <v>5239</v>
       </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
-      <c r="I133" t="inlineStr"/>
-      <c r="J133" t="inlineStr"/>
+      <c r="I133" t="n">
+        <v>5239</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n"/>
@@ -3437,15 +4304,22 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>4453.15</v>
+        <v>5239</v>
       </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="inlineStr"/>
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="inlineStr"/>
-      <c r="I134" t="inlineStr"/>
-      <c r="J134" t="inlineStr"/>
+      <c r="I134" t="n">
+        <v>5239</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
@@ -3490,6 +4364,7 @@
       </c>
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n"/>
@@ -3499,7 +4374,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>6361.4</v>
+        <v>7484</v>
       </c>
       <c r="D136" t="n">
         <v>4500</v>
@@ -3516,8 +4391,15 @@
       <c r="H136" t="n">
         <v>3900</v>
       </c>
-      <c r="I136" t="inlineStr"/>
-      <c r="J136" t="inlineStr"/>
+      <c r="I136" t="n">
+        <v>3470</v>
+      </c>
+      <c r="J136" t="n">
+        <v>4014</v>
+      </c>
+      <c r="K136" t="n">
+        <v>53.63442009620524</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n"/>
@@ -3527,7 +4409,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>6043.5</v>
+        <v>7110</v>
       </c>
       <c r="D137" t="n">
         <v>4500</v>
@@ -3544,8 +4426,15 @@
       <c r="H137" t="n">
         <v>3900</v>
       </c>
-      <c r="I137" t="inlineStr"/>
-      <c r="J137" t="inlineStr"/>
+      <c r="I137" t="n">
+        <v>3470</v>
+      </c>
+      <c r="J137" t="n">
+        <v>3640</v>
+      </c>
+      <c r="K137" t="n">
+        <v>51.19549929676512</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n"/>
@@ -3555,7 +4444,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5725.599999999999</v>
+        <v>6736</v>
       </c>
       <c r="D138" t="n">
         <v>4100</v>
@@ -3572,8 +4461,15 @@
       <c r="H138" t="n">
         <v>3700</v>
       </c>
-      <c r="I138" t="inlineStr"/>
-      <c r="J138" t="inlineStr"/>
+      <c r="I138" t="n">
+        <v>3470</v>
+      </c>
+      <c r="J138" t="n">
+        <v>3266</v>
+      </c>
+      <c r="K138" t="n">
+        <v>48.48574821852731</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n"/>
@@ -3583,7 +4479,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>5089.8</v>
+        <v>5988</v>
       </c>
       <c r="D139" t="n">
         <v>4100</v>
@@ -3600,8 +4496,15 @@
       <c r="H139" t="n">
         <v>3700</v>
       </c>
-      <c r="I139" t="inlineStr"/>
-      <c r="J139" t="inlineStr"/>
+      <c r="I139" t="n">
+        <v>3470</v>
+      </c>
+      <c r="J139" t="n">
+        <v>2518</v>
+      </c>
+      <c r="K139" t="n">
+        <v>42.05076820307281</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n"/>
@@ -3611,7 +4514,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>4453.15</v>
+        <v>5239</v>
       </c>
       <c r="D140" t="n">
         <v>4100</v>
@@ -3628,8 +4531,15 @@
       <c r="H140" t="n">
         <v>2700</v>
       </c>
-      <c r="I140" t="inlineStr"/>
-      <c r="J140" t="inlineStr"/>
+      <c r="I140" t="n">
+        <v>2700</v>
+      </c>
+      <c r="J140" t="n">
+        <v>2539</v>
+      </c>
+      <c r="K140" t="n">
+        <v>48.46344722275243</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n"/>
@@ -3639,7 +4549,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>4453.15</v>
+        <v>5239</v>
       </c>
       <c r="D141" t="n">
         <v>3700</v>
@@ -3648,7 +4558,7 @@
         <v>4674.17</v>
       </c>
       <c r="F141" t="n">
-        <v>3260</v>
+        <v>3492</v>
       </c>
       <c r="G141" t="n">
         <v>3870</v>
@@ -3656,8 +4566,15 @@
       <c r="H141" t="n">
         <v>2700</v>
       </c>
-      <c r="I141" t="inlineStr"/>
-      <c r="J141" t="inlineStr"/>
+      <c r="I141" t="n">
+        <v>2700</v>
+      </c>
+      <c r="J141" t="n">
+        <v>2539</v>
+      </c>
+      <c r="K141" t="n">
+        <v>48.46344722275243</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
@@ -3698,6 +4615,7 @@
       <c r="H142" t="inlineStr"/>
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n"/>
@@ -3707,7 +4625,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>5788.5</v>
+        <v>6810</v>
       </c>
       <c r="D143" t="n">
         <v>9000</v>
@@ -3722,8 +4640,15 @@
         <v>8670</v>
       </c>
       <c r="H143" t="inlineStr"/>
-      <c r="I143" t="inlineStr"/>
-      <c r="J143" t="inlineStr"/>
+      <c r="I143" t="n">
+        <v>6810</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n"/>
@@ -3733,7 +4658,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>5499.5</v>
+        <v>6470</v>
       </c>
       <c r="D144" t="n">
         <v>9000</v>
@@ -3748,8 +4673,15 @@
         <v>8170</v>
       </c>
       <c r="H144" t="inlineStr"/>
-      <c r="I144" t="inlineStr"/>
-      <c r="J144" t="inlineStr"/>
+      <c r="I144" t="n">
+        <v>6470</v>
+      </c>
+      <c r="J144" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n"/>
@@ -3759,7 +4691,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>5209.65</v>
+        <v>6129</v>
       </c>
       <c r="D145" t="n">
         <v>8500</v>
@@ -3774,8 +4706,15 @@
         <v>7470</v>
       </c>
       <c r="H145" t="inlineStr"/>
-      <c r="I145" t="inlineStr"/>
-      <c r="J145" t="inlineStr"/>
+      <c r="I145" t="n">
+        <v>6129</v>
+      </c>
+      <c r="J145" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n"/>
@@ -3785,7 +4724,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>4630.8</v>
+        <v>5448</v>
       </c>
       <c r="D146" t="n">
         <v>8500</v>
@@ -3800,8 +4739,15 @@
         <v>7470</v>
       </c>
       <c r="H146" t="inlineStr"/>
-      <c r="I146" t="inlineStr"/>
-      <c r="J146" t="inlineStr"/>
+      <c r="I146" t="n">
+        <v>5448</v>
+      </c>
+      <c r="J146" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n"/>
@@ -3811,7 +4757,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>4051.95</v>
+        <v>4767</v>
       </c>
       <c r="D147" t="n">
         <v>8500</v>
@@ -3826,8 +4772,15 @@
         <v>6970</v>
       </c>
       <c r="H147" t="inlineStr"/>
-      <c r="I147" t="inlineStr"/>
-      <c r="J147" t="inlineStr"/>
+      <c r="I147" t="n">
+        <v>4767</v>
+      </c>
+      <c r="J147" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n"/>
@@ -3837,7 +4790,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>4051.95</v>
+        <v>4767</v>
       </c>
       <c r="D148" t="n">
         <v>7500</v>
@@ -3852,8 +4805,15 @@
         <v>6970</v>
       </c>
       <c r="H148" t="inlineStr"/>
-      <c r="I148" t="inlineStr"/>
-      <c r="J148" t="inlineStr"/>
+      <c r="I148" t="n">
+        <v>4767</v>
+      </c>
+      <c r="J148" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
@@ -3874,6 +4834,7 @@
       <c r="H149" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n"/>
@@ -3883,15 +4844,22 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>7235.2</v>
+        <v>8512</v>
       </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
       <c r="F150" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr"/>
-      <c r="I150" t="inlineStr"/>
-      <c r="J150" t="inlineStr"/>
+      <c r="I150" t="n">
+        <v>8512</v>
+      </c>
+      <c r="J150" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n"/>
@@ -3901,15 +4869,22 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>6873.95</v>
+        <v>8087</v>
       </c>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
       <c r="F151" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr"/>
-      <c r="I151" t="inlineStr"/>
-      <c r="J151" t="inlineStr"/>
+      <c r="I151" t="n">
+        <v>8087</v>
+      </c>
+      <c r="J151" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n"/>
@@ -3919,15 +4894,22 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>6511.849999999999</v>
+        <v>7661</v>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
       <c r="F152" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="inlineStr"/>
-      <c r="I152" t="inlineStr"/>
-      <c r="J152" t="inlineStr"/>
+      <c r="I152" t="n">
+        <v>7661</v>
+      </c>
+      <c r="J152" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n"/>
@@ -3937,15 +4919,22 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>5788.5</v>
+        <v>6810</v>
       </c>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
       <c r="F153" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="inlineStr"/>
-      <c r="I153" t="inlineStr"/>
-      <c r="J153" t="inlineStr"/>
+      <c r="I153" t="n">
+        <v>6810</v>
+      </c>
+      <c r="J153" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n"/>
@@ -3955,15 +4944,22 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>5065.15</v>
+        <v>5959</v>
       </c>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr"/>
       <c r="F154" t="inlineStr"/>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr"/>
-      <c r="I154" t="inlineStr"/>
-      <c r="J154" t="inlineStr"/>
+      <c r="I154" t="n">
+        <v>5959</v>
+      </c>
+      <c r="J154" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n"/>
@@ -3973,15 +4969,22 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>5065.15</v>
+        <v>5959</v>
       </c>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="inlineStr"/>
       <c r="F155" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr"/>
-      <c r="I155" t="inlineStr"/>
-      <c r="J155" t="inlineStr"/>
+      <c r="I155" t="n">
+        <v>5959</v>
+      </c>
+      <c r="J155" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="22">

</xml_diff>

<commit_message>
step 3 - car names in the result, DELTA column is rounded + sheet name is tie stamp
</commit_message>
<xml_diff>
--- a/outputs/analysiss.xlsx
+++ b/outputs/analysiss.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="not in the list cars" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="05-03-2024@2134" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,6 +447,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>company_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>inspire_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>insp_sipp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>park</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Voyah Free</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Zeekr 001</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Zeekr 009</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jaguar XE ВК49865</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -472,27 +554,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RENT-MOTORS-01-03-24</t>
+          <t>RENT-MOTORS-05-03-24</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>REX-RENT-01-03-24</t>
+          <t>REX-RENT-05-03-24</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>A-ARENDA-01-03-24</t>
+          <t>A-ARENDA-05-03-24</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ALMAK-01-03-24</t>
+          <t>ALMAK-05-03-24</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>STORLET-01-03-24</t>
+          <t>STORLET-05-03-24</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -548,7 +630,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2634</v>
+        <v>2238.9</v>
       </c>
       <c r="D3" t="n">
         <v>1750</v>
@@ -561,10 +643,10 @@
         <v>1750</v>
       </c>
       <c r="J3" t="n">
-        <v>884</v>
+        <v>488.9000000000001</v>
       </c>
       <c r="K3" t="n">
-        <v>33.56112376613515</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="4">
@@ -575,7 +657,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2503</v>
+        <v>2127.55</v>
       </c>
       <c r="D4" t="n">
         <v>1750</v>
@@ -588,10 +670,10 @@
         <v>1750</v>
       </c>
       <c r="J4" t="n">
-        <v>753</v>
+        <v>377.5499999999997</v>
       </c>
       <c r="K4" t="n">
-        <v>30.08389932081502</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="5">
@@ -602,7 +684,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2371</v>
+        <v>2015.35</v>
       </c>
       <c r="D5" t="n">
         <v>1500</v>
@@ -615,10 +697,10 @@
         <v>1500</v>
       </c>
       <c r="J5" t="n">
-        <v>871</v>
+        <v>515.3499999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>36.73555461830451</v>
+        <v>25.57</v>
       </c>
     </row>
     <row r="6">
@@ -629,7 +711,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2187</v>
+        <v>1858.95</v>
       </c>
       <c r="D6" t="n">
         <v>1500</v>
@@ -642,10 +724,10 @@
         <v>1500</v>
       </c>
       <c r="J6" t="n">
-        <v>687</v>
+        <v>358.95</v>
       </c>
       <c r="K6" t="n">
-        <v>31.41289437585734</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="7">
@@ -656,7 +738,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2055</v>
+        <v>1746.75</v>
       </c>
       <c r="D7" t="n">
         <v>1500</v>
@@ -669,10 +751,10 @@
         <v>1500</v>
       </c>
       <c r="J7" t="n">
-        <v>555</v>
+        <v>246.75</v>
       </c>
       <c r="K7" t="n">
-        <v>27.00729927007299</v>
+        <v>14.13</v>
       </c>
     </row>
     <row r="8">
@@ -683,7 +765,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1976</v>
+        <v>1679.6</v>
       </c>
       <c r="D8" t="n">
         <v>1450</v>
@@ -696,10 +778,10 @@
         <v>1450</v>
       </c>
       <c r="J8" t="n">
-        <v>526</v>
+        <v>229.5999999999999</v>
       </c>
       <c r="K8" t="n">
-        <v>26.61943319838057</v>
+        <v>13.67</v>
       </c>
     </row>
     <row r="9">
@@ -731,7 +813,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3292</v>
+        <v>2798.2</v>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -739,7 +821,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>3292</v>
+        <v>2798.2</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -756,7 +838,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3128</v>
+        <v>2658.8</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -764,7 +846,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>3128</v>
+        <v>2658.8</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -781,7 +863,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2963</v>
+        <v>2518.55</v>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -789,7 +871,7 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>2963</v>
+        <v>2518.55</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -806,7 +888,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2733</v>
+        <v>2323.05</v>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
@@ -814,7 +896,7 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
-        <v>2733</v>
+        <v>2323.05</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -831,7 +913,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2568</v>
+        <v>2182.8</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -839,7 +921,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>2568</v>
+        <v>2182.8</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -856,7 +938,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2469</v>
+        <v>2098.65</v>
       </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
@@ -864,7 +946,7 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>2469</v>
+        <v>2098.65</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -1069,7 +1151,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3859</v>
+        <v>3280.15</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -1079,13 +1161,13 @@
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>3470</v>
+        <v>3280.15</v>
       </c>
       <c r="J24" t="n">
-        <v>389</v>
+        <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>10.08033169214823</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1096,7 +1178,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3667</v>
+        <v>3116.95</v>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
@@ -1106,13 +1188,13 @@
       </c>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>3270</v>
+        <v>3116.95</v>
       </c>
       <c r="J25" t="n">
-        <v>397</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>10.82628851922552</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1123,7 +1205,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3474</v>
+        <v>2952.9</v>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
@@ -1133,13 +1215,13 @@
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
-        <v>2970</v>
+        <v>2952.9</v>
       </c>
       <c r="J26" t="n">
-        <v>504</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>14.50777202072539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1150,7 +1232,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3088</v>
+        <v>2624.8</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
@@ -1160,13 +1242,13 @@
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
-        <v>2970</v>
+        <v>2624.8</v>
       </c>
       <c r="J27" t="n">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>3.821243523316062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1177,7 +1259,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2702</v>
+        <v>2296.7</v>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
@@ -1187,7 +1269,7 @@
       </c>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>2702</v>
+        <v>2296.7</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
@@ -1204,7 +1286,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2702</v>
+        <v>2296.7</v>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
@@ -1214,7 +1296,7 @@
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>2702</v>
+        <v>2296.7</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1256,7 +1338,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2861</v>
+        <v>2288.8</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
@@ -1264,7 +1346,7 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>2861</v>
+        <v>2288.8</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -1281,7 +1363,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2718</v>
+        <v>2174.4</v>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
@@ -1289,7 +1371,7 @@
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>2718</v>
+        <v>2174.4</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -1306,7 +1388,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2575</v>
+        <v>2060</v>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
@@ -1314,7 +1396,7 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>2575</v>
+        <v>2060</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
@@ -1331,7 +1413,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2375</v>
+        <v>1900</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -1339,7 +1421,7 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>2375</v>
+        <v>1900</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -1356,7 +1438,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2232</v>
+        <v>1785.6</v>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
@@ -1364,7 +1446,7 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
-        <v>2232</v>
+        <v>1785.6</v>
       </c>
       <c r="J35" t="n">
         <v>0</v>
@@ -1381,7 +1463,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2146</v>
+        <v>1716.8</v>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
@@ -1389,7 +1471,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
-        <v>2146</v>
+        <v>1716.8</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
@@ -1451,7 +1533,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3576</v>
+        <v>2860.8</v>
       </c>
       <c r="D38" t="n">
         <v>2200</v>
@@ -1472,10 +1554,10 @@
         <v>2000</v>
       </c>
       <c r="J38" t="n">
-        <v>1576</v>
+        <v>860.8000000000002</v>
       </c>
       <c r="K38" t="n">
-        <v>44.07158836689038</v>
+        <v>30.09</v>
       </c>
     </row>
     <row r="39">
@@ -1486,7 +1568,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3398</v>
+        <v>2718.4</v>
       </c>
       <c r="D39" t="n">
         <v>2200</v>
@@ -1507,10 +1589,10 @@
         <v>2000</v>
       </c>
       <c r="J39" t="n">
-        <v>1398</v>
+        <v>718.4000000000001</v>
       </c>
       <c r="K39" t="n">
-        <v>41.14184814596822</v>
+        <v>26.43</v>
       </c>
     </row>
     <row r="40">
@@ -1521,7 +1603,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3219</v>
+        <v>2575.2</v>
       </c>
       <c r="D40" t="n">
         <v>1900</v>
@@ -1542,10 +1624,10 @@
         <v>1800</v>
       </c>
       <c r="J40" t="n">
-        <v>1419</v>
+        <v>775.2000000000003</v>
       </c>
       <c r="K40" t="n">
-        <v>44.08201304753029</v>
+        <v>30.1</v>
       </c>
     </row>
     <row r="41">
@@ -1556,7 +1638,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2969</v>
+        <v>2375.2</v>
       </c>
       <c r="D41" t="n">
         <v>1900</v>
@@ -1577,10 +1659,10 @@
         <v>1800</v>
       </c>
       <c r="J41" t="n">
-        <v>1169</v>
+        <v>575.2000000000003</v>
       </c>
       <c r="K41" t="n">
-        <v>39.37352643987875</v>
+        <v>24.22</v>
       </c>
     </row>
     <row r="42">
@@ -1591,7 +1673,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2790</v>
+        <v>2232</v>
       </c>
       <c r="D42" t="n">
         <v>1900</v>
@@ -1612,10 +1694,10 @@
         <v>1500</v>
       </c>
       <c r="J42" t="n">
-        <v>1290</v>
+        <v>732</v>
       </c>
       <c r="K42" t="n">
-        <v>46.23655913978494</v>
+        <v>32.8</v>
       </c>
     </row>
     <row r="43">
@@ -1626,7 +1708,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2682</v>
+        <v>2145.6</v>
       </c>
       <c r="D43" t="n">
         <v>1800</v>
@@ -1635,7 +1717,7 @@
         <v>2216.67</v>
       </c>
       <c r="F43" t="n">
-        <v>2438</v>
+        <v>2424.33</v>
       </c>
       <c r="G43" t="n">
         <v>2170</v>
@@ -1647,10 +1729,10 @@
         <v>1500</v>
       </c>
       <c r="J43" t="n">
-        <v>1182</v>
+        <v>645.5999999999999</v>
       </c>
       <c r="K43" t="n">
-        <v>44.07158836689038</v>
+        <v>30.09</v>
       </c>
     </row>
     <row r="44">
@@ -1686,7 +1768,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3305</v>
+        <v>1983</v>
       </c>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
@@ -1694,7 +1776,7 @@
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="n">
-        <v>3305</v>
+        <v>1983</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
@@ -1711,7 +1793,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3140</v>
+        <v>1884</v>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
@@ -1719,7 +1801,7 @@
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="n">
-        <v>3140</v>
+        <v>1884</v>
       </c>
       <c r="J46" t="n">
         <v>0</v>
@@ -1736,7 +1818,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2975</v>
+        <v>1785</v>
       </c>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
@@ -1744,7 +1826,7 @@
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="n">
-        <v>2975</v>
+        <v>1785</v>
       </c>
       <c r="J47" t="n">
         <v>0</v>
@@ -1761,7 +1843,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2644</v>
+        <v>1586.4</v>
       </c>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
@@ -1769,7 +1851,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="n">
-        <v>2644</v>
+        <v>1586.4</v>
       </c>
       <c r="J48" t="n">
         <v>0</v>
@@ -1786,7 +1868,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>2314</v>
+        <v>1388.4</v>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
@@ -1794,7 +1876,7 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="n">
-        <v>2314</v>
+        <v>1388.4</v>
       </c>
       <c r="J49" t="n">
         <v>0</v>
@@ -1811,7 +1893,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2314</v>
+        <v>1388.4</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
@@ -1819,7 +1901,7 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="n">
-        <v>2314</v>
+        <v>1388.4</v>
       </c>
       <c r="J50" t="n">
         <v>0</v>
@@ -1873,7 +1955,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4131</v>
+        <v>2478.6</v>
       </c>
       <c r="D52" t="n">
         <v>1950</v>
@@ -1890,10 +1972,10 @@
         <v>1800</v>
       </c>
       <c r="J52" t="n">
-        <v>2331</v>
+        <v>678.5999999999999</v>
       </c>
       <c r="K52" t="n">
-        <v>56.42701525054466</v>
+        <v>27.38</v>
       </c>
     </row>
     <row r="53">
@@ -1904,7 +1986,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3925</v>
+        <v>2355</v>
       </c>
       <c r="D53" t="n">
         <v>1950</v>
@@ -1921,10 +2003,10 @@
         <v>1800</v>
       </c>
       <c r="J53" t="n">
-        <v>2125</v>
+        <v>555</v>
       </c>
       <c r="K53" t="n">
-        <v>54.14012738853503</v>
+        <v>23.57</v>
       </c>
     </row>
     <row r="54">
@@ -1935,7 +2017,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3718</v>
+        <v>2230.8</v>
       </c>
       <c r="D54" t="n">
         <v>1700</v>
@@ -1952,10 +2034,10 @@
         <v>1600</v>
       </c>
       <c r="J54" t="n">
-        <v>2118</v>
+        <v>630.7999999999997</v>
       </c>
       <c r="K54" t="n">
-        <v>56.96611081226466</v>
+        <v>28.28</v>
       </c>
     </row>
     <row r="55">
@@ -1966,7 +2048,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3305</v>
+        <v>1983</v>
       </c>
       <c r="D55" t="n">
         <v>1700</v>
@@ -1983,10 +2065,10 @@
         <v>1600</v>
       </c>
       <c r="J55" t="n">
-        <v>1705</v>
+        <v>383</v>
       </c>
       <c r="K55" t="n">
-        <v>51.58850226928896</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="56">
@@ -1997,7 +2079,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2892</v>
+        <v>1735.2</v>
       </c>
       <c r="D56" t="n">
         <v>1700</v>
@@ -2014,10 +2096,10 @@
         <v>1400</v>
       </c>
       <c r="J56" t="n">
-        <v>1492</v>
+        <v>335.2</v>
       </c>
       <c r="K56" t="n">
-        <v>51.59059474412172</v>
+        <v>19.32</v>
       </c>
     </row>
     <row r="57">
@@ -2028,7 +2110,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2892</v>
+        <v>1735.2</v>
       </c>
       <c r="D57" t="n">
         <v>1600</v>
@@ -2045,10 +2127,10 @@
         <v>1400</v>
       </c>
       <c r="J57" t="n">
-        <v>1492</v>
+        <v>335.2</v>
       </c>
       <c r="K57" t="n">
-        <v>51.59059474412172</v>
+        <v>19.32</v>
       </c>
     </row>
     <row r="58">
@@ -2092,7 +2174,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3690</v>
+        <v>3136.5</v>
       </c>
       <c r="D59" t="n">
         <v>3000</v>
@@ -2107,10 +2189,10 @@
         <v>1800</v>
       </c>
       <c r="J59" t="n">
-        <v>1890</v>
+        <v>1336.5</v>
       </c>
       <c r="K59" t="n">
-        <v>51.21951219512195</v>
+        <v>42.61</v>
       </c>
     </row>
     <row r="60">
@@ -2121,7 +2203,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>3506</v>
+        <v>2980.1</v>
       </c>
       <c r="D60" t="n">
         <v>3000</v>
@@ -2136,10 +2218,10 @@
         <v>1800</v>
       </c>
       <c r="J60" t="n">
-        <v>1706</v>
+        <v>1180.1</v>
       </c>
       <c r="K60" t="n">
-        <v>48.6594409583571</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="61">
@@ -2150,7 +2232,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>3321</v>
+        <v>2822.85</v>
       </c>
       <c r="D61" t="n">
         <v>2600</v>
@@ -2165,10 +2247,10 @@
         <v>1600</v>
       </c>
       <c r="J61" t="n">
-        <v>1721</v>
+        <v>1222.85</v>
       </c>
       <c r="K61" t="n">
-        <v>51.82174043962662</v>
+        <v>43.32</v>
       </c>
     </row>
     <row r="62">
@@ -2179,7 +2261,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2952</v>
+        <v>2509.2</v>
       </c>
       <c r="D62" t="n">
         <v>2600</v>
@@ -2194,10 +2276,10 @@
         <v>1600</v>
       </c>
       <c r="J62" t="n">
-        <v>1352</v>
+        <v>909.1999999999998</v>
       </c>
       <c r="K62" t="n">
-        <v>45.79945799457995</v>
+        <v>36.23</v>
       </c>
     </row>
     <row r="63">
@@ -2208,7 +2290,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2583</v>
+        <v>2195.55</v>
       </c>
       <c r="D63" t="n">
         <v>2600</v>
@@ -2223,10 +2305,10 @@
         <v>1200</v>
       </c>
       <c r="J63" t="n">
-        <v>1383</v>
+        <v>995.5499999999997</v>
       </c>
       <c r="K63" t="n">
-        <v>53.54239256678282</v>
+        <v>45.34</v>
       </c>
     </row>
     <row r="64">
@@ -2237,7 +2319,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2583</v>
+        <v>2195.55</v>
       </c>
       <c r="D64" t="n">
         <v>2100</v>
@@ -2252,10 +2334,10 @@
         <v>1200</v>
       </c>
       <c r="J64" t="n">
-        <v>1383</v>
+        <v>995.5499999999997</v>
       </c>
       <c r="K64" t="n">
-        <v>53.54239256678282</v>
+        <v>45.34</v>
       </c>
     </row>
     <row r="65">
@@ -2299,7 +2381,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>4341</v>
+        <v>3689.85</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
@@ -2314,10 +2396,10 @@
         <v>2100</v>
       </c>
       <c r="J66" t="n">
-        <v>2241</v>
+        <v>1589.85</v>
       </c>
       <c r="K66" t="n">
-        <v>51.62404975812025</v>
+        <v>43.09</v>
       </c>
     </row>
     <row r="67">
@@ -2328,7 +2410,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4124</v>
+        <v>3505.4</v>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
@@ -2343,10 +2425,10 @@
         <v>2100</v>
       </c>
       <c r="J67" t="n">
-        <v>2024</v>
+        <v>1405.4</v>
       </c>
       <c r="K67" t="n">
-        <v>49.07856450048497</v>
+        <v>40.09</v>
       </c>
     </row>
     <row r="68">
@@ -2357,7 +2439,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>3907</v>
+        <v>3320.95</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
@@ -2372,10 +2454,10 @@
         <v>1900</v>
       </c>
       <c r="J68" t="n">
-        <v>2007</v>
+        <v>1420.95</v>
       </c>
       <c r="K68" t="n">
-        <v>51.36933708727924</v>
+        <v>42.79</v>
       </c>
     </row>
     <row r="69">
@@ -2386,7 +2468,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3473</v>
+        <v>2952.05</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
@@ -2401,10 +2483,10 @@
         <v>1900</v>
       </c>
       <c r="J69" t="n">
-        <v>1573</v>
+        <v>1052.05</v>
       </c>
       <c r="K69" t="n">
-        <v>45.29225453498416</v>
+        <v>35.64</v>
       </c>
     </row>
     <row r="70">
@@ -2415,7 +2497,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>3039</v>
+        <v>2583.15</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
@@ -2430,10 +2512,10 @@
         <v>1500</v>
       </c>
       <c r="J70" t="n">
-        <v>1539</v>
+        <v>1083.15</v>
       </c>
       <c r="K70" t="n">
-        <v>50.6416584402764</v>
+        <v>41.93</v>
       </c>
     </row>
     <row r="71">
@@ -2444,7 +2526,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3039</v>
+        <v>2583.15</v>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
@@ -2459,10 +2541,10 @@
         <v>1500</v>
       </c>
       <c r="J71" t="n">
-        <v>1539</v>
+        <v>1083.15</v>
       </c>
       <c r="K71" t="n">
-        <v>50.6416584402764</v>
+        <v>41.93</v>
       </c>
     </row>
     <row r="72">
@@ -2488,7 +2570,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>KIA K5 / Hyundai Sonata</t>
+          <t>Chery Arrizo 8</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -2518,7 +2600,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>5001</v>
+        <v>4250.849999999999</v>
       </c>
       <c r="D73" t="n">
         <v>3800</v>
@@ -2539,10 +2621,10 @@
         <v>2500</v>
       </c>
       <c r="J73" t="n">
-        <v>2501</v>
+        <v>1750.849999999999</v>
       </c>
       <c r="K73" t="n">
-        <v>50.00999800039992</v>
+        <v>41.19</v>
       </c>
     </row>
     <row r="74">
@@ -2553,7 +2635,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>4751</v>
+        <v>4038.35</v>
       </c>
       <c r="D74" t="n">
         <v>3800</v>
@@ -2574,10 +2656,10 @@
         <v>2500</v>
       </c>
       <c r="J74" t="n">
-        <v>2251</v>
+        <v>1538.35</v>
       </c>
       <c r="K74" t="n">
-        <v>47.37949905283098</v>
+        <v>38.09</v>
       </c>
     </row>
     <row r="75">
@@ -2588,7 +2670,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4501</v>
+        <v>3825.85</v>
       </c>
       <c r="D75" t="n">
         <v>3200</v>
@@ -2609,10 +2691,10 @@
         <v>2400</v>
       </c>
       <c r="J75" t="n">
-        <v>2101</v>
+        <v>1425.85</v>
       </c>
       <c r="K75" t="n">
-        <v>46.67851588535881</v>
+        <v>37.27</v>
       </c>
     </row>
     <row r="76">
@@ -2623,7 +2705,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4001</v>
+        <v>3400.85</v>
       </c>
       <c r="D76" t="n">
         <v>3200</v>
@@ -2644,10 +2726,10 @@
         <v>2400</v>
       </c>
       <c r="J76" t="n">
-        <v>1601</v>
+        <v>1000.85</v>
       </c>
       <c r="K76" t="n">
-        <v>40.01499625093727</v>
+        <v>29.43</v>
       </c>
     </row>
     <row r="77">
@@ -2658,7 +2740,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>3501</v>
+        <v>2975.85</v>
       </c>
       <c r="D77" t="n">
         <v>3200</v>
@@ -2679,10 +2761,10 @@
         <v>1900</v>
       </c>
       <c r="J77" t="n">
-        <v>1601</v>
+        <v>1075.85</v>
       </c>
       <c r="K77" t="n">
-        <v>45.72979148814624</v>
+        <v>36.15</v>
       </c>
     </row>
     <row r="78">
@@ -2693,7 +2775,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>3501</v>
+        <v>2975.85</v>
       </c>
       <c r="D78" t="n">
         <v>2800</v>
@@ -2702,7 +2784,7 @@
         <v>4674.17</v>
       </c>
       <c r="F78" t="n">
-        <v>3634</v>
+        <v>3686.33</v>
       </c>
       <c r="G78" t="n">
         <v>3170</v>
@@ -2714,10 +2796,10 @@
         <v>1900</v>
       </c>
       <c r="J78" t="n">
-        <v>1601</v>
+        <v>1075.85</v>
       </c>
       <c r="K78" t="n">
-        <v>45.72979148814624</v>
+        <v>36.15</v>
       </c>
     </row>
     <row r="79">
@@ -2749,7 +2831,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5556</v>
+        <v>4722.599999999999</v>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
@@ -2757,7 +2839,7 @@
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="n">
-        <v>5556</v>
+        <v>4722.599999999999</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
@@ -2774,7 +2856,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5279</v>
+        <v>4487.15</v>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
@@ -2782,7 +2864,7 @@
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="n">
-        <v>5279</v>
+        <v>4487.15</v>
       </c>
       <c r="J81" t="n">
         <v>0</v>
@@ -2799,7 +2881,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>5001</v>
+        <v>4250.849999999999</v>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
@@ -2807,7 +2889,7 @@
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="n">
-        <v>5001</v>
+        <v>4250.849999999999</v>
       </c>
       <c r="J82" t="n">
         <v>0</v>
@@ -2824,7 +2906,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4445</v>
+        <v>3778.25</v>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
@@ -2832,7 +2914,7 @@
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="n">
-        <v>4445</v>
+        <v>3778.25</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
@@ -2849,7 +2931,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3890</v>
+        <v>3306.5</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
@@ -2857,7 +2939,7 @@
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="n">
-        <v>3890</v>
+        <v>3306.5</v>
       </c>
       <c r="J84" t="n">
         <v>0</v>
@@ -2874,7 +2956,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3890</v>
+        <v>3306.5</v>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
@@ -2882,7 +2964,7 @@
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="n">
-        <v>3890</v>
+        <v>3306.5</v>
       </c>
       <c r="J85" t="n">
         <v>0</v>
@@ -2936,7 +3018,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4039</v>
+        <v>3231.2</v>
       </c>
       <c r="D87" t="n">
         <v>3300</v>
@@ -2953,10 +3035,10 @@
         <v>2200</v>
       </c>
       <c r="J87" t="n">
-        <v>1839</v>
+        <v>1031.2</v>
       </c>
       <c r="K87" t="n">
-        <v>45.53107204753652</v>
+        <v>31.91</v>
       </c>
     </row>
     <row r="88">
@@ -2967,7 +3049,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3838</v>
+        <v>3070.4</v>
       </c>
       <c r="D88" t="n">
         <v>3300</v>
@@ -2984,10 +3066,10 @@
         <v>2200</v>
       </c>
       <c r="J88" t="n">
-        <v>1638</v>
+        <v>870.4000000000001</v>
       </c>
       <c r="K88" t="n">
-        <v>42.67847837415321</v>
+        <v>28.35</v>
       </c>
     </row>
     <row r="89">
@@ -2998,7 +3080,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3636</v>
+        <v>2908.8</v>
       </c>
       <c r="D89" t="n">
         <v>2900</v>
@@ -3015,10 +3097,10 @@
         <v>1900</v>
       </c>
       <c r="J89" t="n">
-        <v>1736</v>
+        <v>1008.8</v>
       </c>
       <c r="K89" t="n">
-        <v>47.74477447744774</v>
+        <v>34.68</v>
       </c>
     </row>
     <row r="90">
@@ -3029,7 +3111,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>3232</v>
+        <v>2585.6</v>
       </c>
       <c r="D90" t="n">
         <v>2900</v>
@@ -3046,10 +3128,10 @@
         <v>1900</v>
       </c>
       <c r="J90" t="n">
-        <v>1332</v>
+        <v>685.6000000000004</v>
       </c>
       <c r="K90" t="n">
-        <v>41.21287128712871</v>
+        <v>26.52</v>
       </c>
     </row>
     <row r="91">
@@ -3060,7 +3142,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3030</v>
+        <v>2424</v>
       </c>
       <c r="D91" t="n">
         <v>2900</v>
@@ -3077,10 +3159,10 @@
         <v>1600</v>
       </c>
       <c r="J91" t="n">
-        <v>1430</v>
+        <v>824</v>
       </c>
       <c r="K91" t="n">
-        <v>47.1947194719472</v>
+        <v>33.99</v>
       </c>
     </row>
     <row r="92">
@@ -3091,7 +3173,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2828</v>
+        <v>2262.4</v>
       </c>
       <c r="D92" t="n">
         <v>2200</v>
@@ -3108,10 +3190,10 @@
         <v>1600</v>
       </c>
       <c r="J92" t="n">
-        <v>1228</v>
+        <v>662.4000000000001</v>
       </c>
       <c r="K92" t="n">
-        <v>43.42291371994342</v>
+        <v>29.28</v>
       </c>
     </row>
     <row r="93">
@@ -3155,7 +3237,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>4487</v>
+        <v>3589.6</v>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="n">
@@ -3167,13 +3249,13 @@
       </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="n">
-        <v>3670</v>
+        <v>3589.6</v>
       </c>
       <c r="J94" t="n">
-        <v>817</v>
+        <v>0</v>
       </c>
       <c r="K94" t="n">
-        <v>18.20815689770448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -3184,7 +3266,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>4263</v>
+        <v>3410.4</v>
       </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="n">
@@ -3196,13 +3278,13 @@
       </c>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="n">
-        <v>3470</v>
+        <v>3410.4</v>
       </c>
       <c r="J95" t="n">
-        <v>793</v>
+        <v>0</v>
       </c>
       <c r="K95" t="n">
-        <v>18.6019235280319</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3213,7 +3295,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4039</v>
+        <v>3231.2</v>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="n">
@@ -3228,10 +3310,10 @@
         <v>2871.43</v>
       </c>
       <c r="J96" t="n">
-        <v>1167.57</v>
+        <v>359.7700000000004</v>
       </c>
       <c r="K96" t="n">
-        <v>28.90740282248082</v>
+        <v>11.13</v>
       </c>
     </row>
     <row r="97">
@@ -3242,7 +3324,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>3590</v>
+        <v>2872</v>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
@@ -3257,10 +3339,10 @@
         <v>2835.71</v>
       </c>
       <c r="J97" t="n">
-        <v>754.29</v>
+        <v>36.28999999999996</v>
       </c>
       <c r="K97" t="n">
-        <v>21.0108635097493</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="98">
@@ -3271,7 +3353,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>3366</v>
+        <v>2692.8</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="n">
@@ -3283,13 +3365,13 @@
       </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="n">
-        <v>2823.81</v>
+        <v>2692.8</v>
       </c>
       <c r="J98" t="n">
-        <v>542.1900000000001</v>
+        <v>0</v>
       </c>
       <c r="K98" t="n">
-        <v>16.1078431372549</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -3300,7 +3382,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>3141</v>
+        <v>2512.8</v>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
@@ -3312,13 +3394,13 @@
       </c>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="n">
-        <v>2816.67</v>
+        <v>2512.8</v>
       </c>
       <c r="J99" t="n">
-        <v>324.3299999999999</v>
+        <v>0</v>
       </c>
       <c r="K99" t="n">
-        <v>10.32569245463228</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3530,7 +3612,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>4701</v>
+        <v>3760.8</v>
       </c>
       <c r="D108" t="n">
         <v>3700</v>
@@ -3549,10 +3631,10 @@
         <v>3270</v>
       </c>
       <c r="J108" t="n">
-        <v>1431</v>
+        <v>490.8000000000002</v>
       </c>
       <c r="K108" t="n">
-        <v>30.44033184428845</v>
+        <v>13.05</v>
       </c>
     </row>
     <row r="109">
@@ -3563,7 +3645,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4466</v>
+        <v>3572.8</v>
       </c>
       <c r="D109" t="n">
         <v>3700</v>
@@ -3582,10 +3664,10 @@
         <v>3070</v>
       </c>
       <c r="J109" t="n">
-        <v>1396</v>
+        <v>502.8000000000002</v>
       </c>
       <c r="K109" t="n">
-        <v>31.25839677563815</v>
+        <v>14.07</v>
       </c>
     </row>
     <row r="110">
@@ -3596,7 +3678,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>4231</v>
+        <v>3384.8</v>
       </c>
       <c r="D110" t="n">
         <v>3200</v>
@@ -3615,10 +3697,10 @@
         <v>2870</v>
       </c>
       <c r="J110" t="n">
-        <v>1361</v>
+        <v>514.8000000000002</v>
       </c>
       <c r="K110" t="n">
-        <v>32.16733632710943</v>
+        <v>15.21</v>
       </c>
     </row>
     <row r="111">
@@ -3629,7 +3711,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>3761</v>
+        <v>3008.8</v>
       </c>
       <c r="D111" t="n">
         <v>3200</v>
@@ -3648,10 +3730,10 @@
         <v>2870</v>
       </c>
       <c r="J111" t="n">
-        <v>891</v>
+        <v>138.8000000000002</v>
       </c>
       <c r="K111" t="n">
-        <v>23.6905078436586</v>
+        <v>4.61</v>
       </c>
     </row>
     <row r="112">
@@ -3662,7 +3744,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>3291</v>
+        <v>2632.8</v>
       </c>
       <c r="D112" t="n">
         <v>3200</v>
@@ -3681,10 +3763,10 @@
         <v>2500</v>
       </c>
       <c r="J112" t="n">
-        <v>791</v>
+        <v>132.8000000000002</v>
       </c>
       <c r="K112" t="n">
-        <v>24.03524764509268</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="113">
@@ -3695,14 +3777,14 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>3291</v>
+        <v>2632.8</v>
       </c>
       <c r="D113" t="n">
         <v>2500</v>
       </c>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="n">
-        <v>3192</v>
+        <v>3217.33</v>
       </c>
       <c r="G113" t="n">
         <v>2670</v>
@@ -3714,10 +3796,10 @@
         <v>2500</v>
       </c>
       <c r="J113" t="n">
-        <v>791</v>
+        <v>132.8000000000002</v>
       </c>
       <c r="K113" t="n">
-        <v>24.03524764509268</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="114">
@@ -3749,7 +3831,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>6275</v>
+        <v>3137.5</v>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
@@ -3757,7 +3839,7 @@
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="n">
-        <v>6275</v>
+        <v>3137.5</v>
       </c>
       <c r="J115" t="n">
         <v>0</v>
@@ -3774,7 +3856,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>5962</v>
+        <v>2981</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
@@ -3782,7 +3864,7 @@
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
       <c r="I116" t="n">
-        <v>5962</v>
+        <v>2981</v>
       </c>
       <c r="J116" t="n">
         <v>0</v>
@@ -3799,7 +3881,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>5648</v>
+        <v>2824</v>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
@@ -3807,7 +3889,7 @@
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="n">
-        <v>5648</v>
+        <v>2824</v>
       </c>
       <c r="J117" t="n">
         <v>0</v>
@@ -3824,7 +3906,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>5020</v>
+        <v>2510</v>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
@@ -3832,7 +3914,7 @@
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="n">
-        <v>5020</v>
+        <v>2510</v>
       </c>
       <c r="J118" t="n">
         <v>0</v>
@@ -3849,7 +3931,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>4393</v>
+        <v>2196.5</v>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
@@ -3857,7 +3939,7 @@
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="n">
-        <v>4393</v>
+        <v>2196.5</v>
       </c>
       <c r="J119" t="n">
         <v>0</v>
@@ -3874,7 +3956,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4393</v>
+        <v>2196.5</v>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
@@ -3882,7 +3964,7 @@
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
       <c r="I120" t="n">
-        <v>4393</v>
+        <v>2196.5</v>
       </c>
       <c r="J120" t="n">
         <v>0</v>
@@ -3944,7 +4026,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>6275</v>
+        <v>3137.5</v>
       </c>
       <c r="D122" t="n">
         <v>3700</v>
@@ -3965,10 +4047,10 @@
         <v>2500</v>
       </c>
       <c r="J122" t="n">
-        <v>3775</v>
+        <v>637.5</v>
       </c>
       <c r="K122" t="n">
-        <v>60.1593625498008</v>
+        <v>20.32</v>
       </c>
     </row>
     <row r="123">
@@ -3979,7 +4061,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>5962</v>
+        <v>2981</v>
       </c>
       <c r="D123" t="n">
         <v>3700</v>
@@ -4000,10 +4082,10 @@
         <v>2500</v>
       </c>
       <c r="J123" t="n">
-        <v>3462</v>
+        <v>481</v>
       </c>
       <c r="K123" t="n">
-        <v>58.06776249580678</v>
+        <v>16.14</v>
       </c>
     </row>
     <row r="124">
@@ -4014,7 +4096,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>5648</v>
+        <v>2824</v>
       </c>
       <c r="D124" t="n">
         <v>3300</v>
@@ -4035,10 +4117,10 @@
         <v>2500</v>
       </c>
       <c r="J124" t="n">
-        <v>3148</v>
+        <v>324</v>
       </c>
       <c r="K124" t="n">
-        <v>55.73654390934845</v>
+        <v>11.47</v>
       </c>
     </row>
     <row r="125">
@@ -4049,7 +4131,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>5020</v>
+        <v>2510</v>
       </c>
       <c r="D125" t="n">
         <v>3300</v>
@@ -4070,10 +4152,10 @@
         <v>2500</v>
       </c>
       <c r="J125" t="n">
-        <v>2520</v>
+        <v>10</v>
       </c>
       <c r="K125" t="n">
-        <v>50.19920318725099</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="126">
@@ -4084,7 +4166,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>4393</v>
+        <v>2196.5</v>
       </c>
       <c r="D126" t="n">
         <v>3300</v>
@@ -4102,13 +4184,13 @@
         <v>2500</v>
       </c>
       <c r="I126" t="n">
-        <v>2500</v>
+        <v>2196.5</v>
       </c>
       <c r="J126" t="n">
-        <v>1893</v>
+        <v>0</v>
       </c>
       <c r="K126" t="n">
-        <v>43.09128158433872</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -4119,7 +4201,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4393</v>
+        <v>2196.5</v>
       </c>
       <c r="D127" t="n">
         <v>2800</v>
@@ -4128,7 +4210,7 @@
         <v>2816.67</v>
       </c>
       <c r="F127" t="n">
-        <v>2718</v>
+        <v>2754.33</v>
       </c>
       <c r="G127" t="n">
         <v>3270</v>
@@ -4137,13 +4219,13 @@
         <v>2500</v>
       </c>
       <c r="I127" t="n">
-        <v>2500</v>
+        <v>2196.5</v>
       </c>
       <c r="J127" t="n">
-        <v>1893</v>
+        <v>0</v>
       </c>
       <c r="K127" t="n">
-        <v>43.09128158433872</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -4179,7 +4261,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>7484</v>
+        <v>5987.200000000001</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
@@ -4187,7 +4269,7 @@
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
       <c r="I129" t="n">
-        <v>7484</v>
+        <v>5987.200000000001</v>
       </c>
       <c r="J129" t="n">
         <v>0</v>
@@ -4204,7 +4286,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>7110</v>
+        <v>5688</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
@@ -4212,7 +4294,7 @@
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr"/>
       <c r="I130" t="n">
-        <v>7110</v>
+        <v>5688</v>
       </c>
       <c r="J130" t="n">
         <v>0</v>
@@ -4229,7 +4311,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>6736</v>
+        <v>5388.8</v>
       </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
@@ -4237,7 +4319,7 @@
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
       <c r="I131" t="n">
-        <v>6736</v>
+        <v>5388.8</v>
       </c>
       <c r="J131" t="n">
         <v>0</v>
@@ -4254,7 +4336,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>5988</v>
+        <v>4790.400000000001</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
@@ -4262,7 +4344,7 @@
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr"/>
       <c r="I132" t="n">
-        <v>5988</v>
+        <v>4790.400000000001</v>
       </c>
       <c r="J132" t="n">
         <v>0</v>
@@ -4279,7 +4361,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>5239</v>
+        <v>4191.2</v>
       </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
@@ -4287,7 +4369,7 @@
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
       <c r="I133" t="n">
-        <v>5239</v>
+        <v>4191.2</v>
       </c>
       <c r="J133" t="n">
         <v>0</v>
@@ -4304,7 +4386,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>5239</v>
+        <v>4191.2</v>
       </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
@@ -4312,7 +4394,7 @@
       <c r="G134" t="inlineStr"/>
       <c r="H134" t="inlineStr"/>
       <c r="I134" t="n">
-        <v>5239</v>
+        <v>4191.2</v>
       </c>
       <c r="J134" t="n">
         <v>0</v>
@@ -4374,7 +4456,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>7484</v>
+        <v>5987.200000000001</v>
       </c>
       <c r="D136" t="n">
         <v>4500</v>
@@ -4395,10 +4477,10 @@
         <v>3470</v>
       </c>
       <c r="J136" t="n">
-        <v>4014</v>
+        <v>2517.200000000001</v>
       </c>
       <c r="K136" t="n">
-        <v>53.63442009620524</v>
+        <v>42.04</v>
       </c>
     </row>
     <row r="137">
@@ -4409,7 +4491,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>7110</v>
+        <v>5688</v>
       </c>
       <c r="D137" t="n">
         <v>4500</v>
@@ -4430,10 +4512,10 @@
         <v>3470</v>
       </c>
       <c r="J137" t="n">
-        <v>3640</v>
+        <v>2218</v>
       </c>
       <c r="K137" t="n">
-        <v>51.19549929676512</v>
+        <v>38.99</v>
       </c>
     </row>
     <row r="138">
@@ -4444,7 +4526,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6736</v>
+        <v>5388.8</v>
       </c>
       <c r="D138" t="n">
         <v>4100</v>
@@ -4465,10 +4547,10 @@
         <v>3470</v>
       </c>
       <c r="J138" t="n">
-        <v>3266</v>
+        <v>1918.8</v>
       </c>
       <c r="K138" t="n">
-        <v>48.48574821852731</v>
+        <v>35.61</v>
       </c>
     </row>
     <row r="139">
@@ -4479,7 +4561,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>5988</v>
+        <v>4790.400000000001</v>
       </c>
       <c r="D139" t="n">
         <v>4100</v>
@@ -4500,10 +4582,10 @@
         <v>3470</v>
       </c>
       <c r="J139" t="n">
-        <v>2518</v>
+        <v>1320.400000000001</v>
       </c>
       <c r="K139" t="n">
-        <v>42.05076820307281</v>
+        <v>27.56</v>
       </c>
     </row>
     <row r="140">
@@ -4514,7 +4596,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>5239</v>
+        <v>4191.2</v>
       </c>
       <c r="D140" t="n">
         <v>4100</v>
@@ -4535,10 +4617,10 @@
         <v>2700</v>
       </c>
       <c r="J140" t="n">
-        <v>2539</v>
+        <v>1491.2</v>
       </c>
       <c r="K140" t="n">
-        <v>48.46344722275243</v>
+        <v>35.58</v>
       </c>
     </row>
     <row r="141">
@@ -4549,7 +4631,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>5239</v>
+        <v>4191.2</v>
       </c>
       <c r="D141" t="n">
         <v>3700</v>
@@ -4558,7 +4640,7 @@
         <v>4674.17</v>
       </c>
       <c r="F141" t="n">
-        <v>3492</v>
+        <v>3530.67</v>
       </c>
       <c r="G141" t="n">
         <v>3870</v>
@@ -4570,10 +4652,10 @@
         <v>2700</v>
       </c>
       <c r="J141" t="n">
-        <v>2539</v>
+        <v>1491.2</v>
       </c>
       <c r="K141" t="n">
-        <v>48.46344722275243</v>
+        <v>35.58</v>
       </c>
     </row>
     <row r="142">
@@ -4625,7 +4707,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6810</v>
+        <v>5788.5</v>
       </c>
       <c r="D143" t="n">
         <v>9000</v>
@@ -4641,7 +4723,7 @@
       </c>
       <c r="H143" t="inlineStr"/>
       <c r="I143" t="n">
-        <v>6810</v>
+        <v>5788.5</v>
       </c>
       <c r="J143" t="n">
         <v>0</v>
@@ -4658,7 +4740,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>6470</v>
+        <v>5499.5</v>
       </c>
       <c r="D144" t="n">
         <v>9000</v>
@@ -4674,7 +4756,7 @@
       </c>
       <c r="H144" t="inlineStr"/>
       <c r="I144" t="n">
-        <v>6470</v>
+        <v>5499.5</v>
       </c>
       <c r="J144" t="n">
         <v>0</v>
@@ -4691,7 +4773,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6129</v>
+        <v>5209.65</v>
       </c>
       <c r="D145" t="n">
         <v>8500</v>
@@ -4707,7 +4789,7 @@
       </c>
       <c r="H145" t="inlineStr"/>
       <c r="I145" t="n">
-        <v>6129</v>
+        <v>5209.65</v>
       </c>
       <c r="J145" t="n">
         <v>0</v>
@@ -4724,7 +4806,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5448</v>
+        <v>4630.8</v>
       </c>
       <c r="D146" t="n">
         <v>8500</v>
@@ -4740,7 +4822,7 @@
       </c>
       <c r="H146" t="inlineStr"/>
       <c r="I146" t="n">
-        <v>5448</v>
+        <v>4630.8</v>
       </c>
       <c r="J146" t="n">
         <v>0</v>
@@ -4757,7 +4839,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>4767</v>
+        <v>4051.95</v>
       </c>
       <c r="D147" t="n">
         <v>8500</v>
@@ -4773,7 +4855,7 @@
       </c>
       <c r="H147" t="inlineStr"/>
       <c r="I147" t="n">
-        <v>4767</v>
+        <v>4051.95</v>
       </c>
       <c r="J147" t="n">
         <v>0</v>
@@ -4790,7 +4872,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>4767</v>
+        <v>4051.95</v>
       </c>
       <c r="D148" t="n">
         <v>7500</v>
@@ -4806,7 +4888,7 @@
       </c>
       <c r="H148" t="inlineStr"/>
       <c r="I148" t="n">
-        <v>4767</v>
+        <v>4051.95</v>
       </c>
       <c r="J148" t="n">
         <v>0</v>
@@ -4844,7 +4926,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>8512</v>
+        <v>7235.2</v>
       </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
@@ -4852,7 +4934,7 @@
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr"/>
       <c r="I150" t="n">
-        <v>8512</v>
+        <v>7235.2</v>
       </c>
       <c r="J150" t="n">
         <v>0</v>
@@ -4869,7 +4951,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>8087</v>
+        <v>6873.95</v>
       </c>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
@@ -4877,7 +4959,7 @@
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr"/>
       <c r="I151" t="n">
-        <v>8087</v>
+        <v>6873.95</v>
       </c>
       <c r="J151" t="n">
         <v>0</v>
@@ -4894,7 +4976,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>7661</v>
+        <v>6511.849999999999</v>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
@@ -4902,7 +4984,7 @@
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="inlineStr"/>
       <c r="I152" t="n">
-        <v>7661</v>
+        <v>6511.849999999999</v>
       </c>
       <c r="J152" t="n">
         <v>0</v>
@@ -4919,7 +5001,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>6810</v>
+        <v>5788.5</v>
       </c>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
@@ -4927,7 +5009,7 @@
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="inlineStr"/>
       <c r="I153" t="n">
-        <v>6810</v>
+        <v>5788.5</v>
       </c>
       <c r="J153" t="n">
         <v>0</v>
@@ -4944,7 +5026,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>5959</v>
+        <v>5065.15</v>
       </c>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr"/>
@@ -4952,7 +5034,7 @@
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr"/>
       <c r="I154" t="n">
-        <v>5959</v>
+        <v>5065.15</v>
       </c>
       <c r="J154" t="n">
         <v>0</v>
@@ -4969,7 +5051,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>5959</v>
+        <v>5065.15</v>
       </c>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="inlineStr"/>
@@ -4977,7 +5059,7 @@
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr"/>
       <c r="I155" t="n">
-        <v>5959</v>
+        <v>5065.15</v>
       </c>
       <c r="J155" t="n">
         <v>0</v>

</xml_diff>